<commit_message>
ya esta el errorbar W vs C
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="h1" sheetId="1" state="visible" r:id="rId2"/>
@@ -151,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -165,6 +165,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -187,8 +191,8 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -805,10 +809,10 @@
         <v>2.2</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>1.4</v>
+        <v>0.35</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>113.905159071452</v>
+        <v>28.476</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,10 +1052,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1267,6 +1271,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
       <c r="C13" s="3" t="n">
         <f aca="false">AVERAGE(C2:C12)</f>
         <v>32.0218181818182</v>
@@ -1281,17 +1287,19 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
       <c r="C14" s="3" t="n">
-        <f aca="false">AVEDEV(C2:C12)</f>
-        <v>13.8947107438017</v>
+        <f aca="false">STDEV(C2:C12)</f>
+        <v>16.6060331314747</v>
       </c>
       <c r="D14" s="3" t="n">
-        <f aca="false">AVEDEV(D2:D12)</f>
-        <v>4953.44702945177</v>
+        <f aca="false">STDEV(D2:D12)</f>
+        <v>6222.5817314347</v>
       </c>
       <c r="E14" s="3" t="n">
-        <f aca="false">AVEDEV(E2:E12)</f>
-        <v>7175.61075721797</v>
+        <f aca="false">STDEV(E2:E12)</f>
+        <v>8979.44427514194</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,34 +1473,35 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="2" t="n">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="3" t="n">
         <f aca="false">AVERAGE(C15:C24)</f>
         <v>19.129</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="3" t="n">
         <f aca="false">AVERAGE(D15:D24)</f>
         <v>1577.5339156448</v>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="3" t="n">
         <f aca="false">AVERAGE(E15:E24)</f>
         <v>4812.61366250466</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>1.29158438009571</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>0.00841563</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>3.64249463</v>
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="3" t="n">
+        <f aca="false">STDEV(C15:C24)</f>
+        <v>7.74273774434972</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <f aca="false">STDEV(D15:D24)</f>
+        <v>1802.24136000069</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <f aca="false">STDEV(E15:E24)</f>
+        <v>8342.41579721475</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,13 +1512,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>1.24844559192559</v>
+        <v>1.29158438009571</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>0.0126416</v>
+        <v>0.00841563</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1.0636196</v>
+        <v>3.64249463</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,13 +1529,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.18008381810848</v>
+        <v>1.24844559192559</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0.0122</v>
+        <v>0.0126416</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>5</v>
+        <v>1.0636196</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,13 +1546,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>2.57704093109965</v>
+        <v>0.18008381810848</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>0.0122</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>4.9376285</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,13 +1563,13 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>2.87</v>
+        <v>2.57704093109965</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>1.66351515740336</v>
+        <v>0.0122</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>67.975558876656</v>
+        <v>4.9376285</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,13 +1580,13 @@
         <v>6</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>2.28</v>
+        <v>2.87</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>1.5</v>
+        <v>1.66351515740336</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>120.345257036891</v>
+        <v>67.975558876656</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1588,13 +1597,13 @@
         <v>6</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>2.75</v>
+        <v>2.28</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.87</v>
+        <v>1.5</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>209.929047509172</v>
+        <v>120.345257036891</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,13 +1614,13 @@
         <v>6</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>2.77</v>
+        <v>2.75</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>0.0057</v>
+        <v>0.87</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>36.4192772320191</v>
+        <v>209.929047509172</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,13 +1631,13 @@
         <v>6</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>3.38578079004554</v>
+        <v>2.77</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0</v>
+        <v>0.0057</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>44.6968257675166</v>
+        <v>36.4192772320191</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,13 +1648,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>6.1423685779091</v>
+        <v>3.38578079004554</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>0.65362923110231</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>61.204279218038</v>
+        <v>44.6968257675166</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,13 +1665,13 @@
         <v>6</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>2.12444949144756</v>
+        <v>6.1423685779091</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>0.12860834302005</v>
+        <v>0.65362923110231</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>111.358991000705</v>
+        <v>61.204279218038</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,13 +1682,13 @@
         <v>6</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>1.64372830981383</v>
+        <v>2.12444949144756</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>1.23110426412406</v>
+        <v>0.12860834302005</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>52.4697529734385</v>
+        <v>111.358991000705</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,61 +1699,62 @@
         <v>6</v>
       </c>
       <c r="C38" s="2" t="n">
+        <v>1.64372830981383</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>1.23110426412406</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>52.4697529734385</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="n">
         <v>1.64174977502717</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D39" s="2" t="n">
         <v>0.205105039964668</v>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E39" s="2" t="n">
         <v>9.88817275910025</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="2" t="n">
-        <f aca="false">AVERAGE(C26:C38)</f>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="3" t="n">
+        <f aca="false">AVERAGE(C27:C39)</f>
         <v>2.37732551272866</v>
       </c>
-      <c r="D39" s="2" t="n">
-        <f aca="false">AVERAGE(D26:D38)</f>
+      <c r="D40" s="3" t="n">
+        <f aca="false">AVERAGE(D27:D39)</f>
         <v>0.484855328124188</v>
       </c>
-      <c r="E39" s="2" t="n">
-        <f aca="false">AVERAGE(E26:E38)</f>
+      <c r="E40" s="3" t="n">
+        <f aca="false">AVERAGE(E27:E39)</f>
         <v>56.0716080848874</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="2" t="n">
-        <v>1.23459490563882</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>0.364</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>69.962389</v>
-      </c>
-    </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="2" t="n">
-        <v>0.126208050958238</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>0.13845</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>31.7354018</v>
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="3" t="n">
+        <f aca="false">STDEV(C27:C39)</f>
+        <v>1.42015125547183</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <f aca="false">STDEV(D27:D39)</f>
+        <v>0.62716954022705</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <f aca="false">STDEV(E27:E39)</f>
+        <v>61.0239865938885</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,13 +1765,13 @@
         <v>7</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>2.32294719616655</v>
+        <v>1.23459490563882</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>0.7545</v>
+        <v>0.364</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>89.3505</v>
+        <v>69.962389</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,13 +1782,13 @@
         <v>7</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>1.86686338186226</v>
+        <v>0.126208050958238</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0.512</v>
+        <v>0.13845</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>74.15866</v>
+        <v>31.7354018</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,13 +1799,13 @@
         <v>7</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>0.68</v>
+        <v>2.32294719616655</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0.48</v>
+        <v>0.7545</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>17.7678461917401</v>
+        <v>89.3505</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,13 +1816,13 @@
         <v>7</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>0.49</v>
+        <v>1.86686338186226</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>0.0174651905815287</v>
+        <v>0.512</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>2.95156203066362</v>
+        <v>74.15866</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,13 +1833,13 @@
         <v>7</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>2.2</v>
+        <v>0.68</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>1.4</v>
+        <v>0.48</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>113.905159071452</v>
+        <v>17.7678461917401</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,13 +1850,13 @@
         <v>7</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>1.29397494095473</v>
+        <v>0.49</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>0.157966917009894</v>
+        <v>0.0174651905815287</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>42.5849619103327</v>
+        <v>2.95156203066362</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,13 +1867,13 @@
         <v>7</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>0.939054273745895</v>
+        <v>2.2</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>0.642678276399</v>
+        <v>0.35</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>26.1916144346342</v>
+        <v>28.476</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,13 +1884,13 @@
         <v>7</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>1.60567008185065</v>
+        <v>1.29397494095473</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>0.0468030657792558</v>
+        <v>0.157966917009894</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>9.36449816889258</v>
+        <v>42.5849619103327</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,13 +1901,13 @@
         <v>7</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>0.641473347043481</v>
+        <v>0.939054273745895</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>0.0331384376767369</v>
+        <v>0.642678276399</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>8.54009763575133</v>
+        <v>26.1916144346342</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,13 +1918,13 @@
         <v>7</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>5.84340792445856</v>
+        <v>1.60567008185065</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>0.0142678859297363</v>
+        <v>0.0468030657792558</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>11.521276814055</v>
+        <v>9.36449816889258</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,13 +1935,13 @@
         <v>7</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>1.14</v>
+        <v>0.641473347043481</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>0.075828523789501</v>
+        <v>0.0331384376767369</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>8.9201006853364</v>
+        <v>8.54009763575133</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,27 +1952,75 @@
         <v>7</v>
       </c>
       <c r="C53" s="2" t="n">
+        <v>5.84340792445856</v>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>0.0142678859297363</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>11.521276814055</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>0.075828523789501</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>8.9201006853364</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="2" t="n">
         <v>1.30512358500124</v>
       </c>
-      <c r="D53" s="2" t="n">
+      <c r="D55" s="2" t="n">
         <v>0.1288315905977</v>
       </c>
-      <c r="E53" s="2" t="n">
+      <c r="E55" s="2" t="n">
         <v>74.756354115002</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="1" t="n">
-        <f aca="false">AVERAGE(C40:C53)</f>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="4" t="n">
+        <f aca="false">AVERAGE(C42:C55)</f>
         <v>1.54923697769146</v>
       </c>
-      <c r="D54" s="1" t="n">
-        <f aca="false">AVERAGE(D40:D53)</f>
-        <v>0.340423563411668</v>
-      </c>
-      <c r="E54" s="1" t="n">
-        <f aca="false">AVERAGE(E40:E53)</f>
-        <v>41.5507444184186</v>
+      <c r="D56" s="4" t="n">
+        <f aca="false">AVERAGE(D42:D55)</f>
+        <v>0.265423563411668</v>
+      </c>
+      <c r="E56" s="4" t="n">
+        <f aca="false">AVERAGE(E42:E55)</f>
+        <v>35.4486616276006</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="4" t="n">
+        <f aca="false">STDEV(C42:C55)</f>
+        <v>1.38830956757735</v>
+      </c>
+      <c r="D57" s="4" t="n">
+        <f aca="false">STDEV(D42:D55)</f>
+        <v>0.250202540470363</v>
+      </c>
+      <c r="E57" s="4" t="n">
+        <f aca="false">STDEV(E42:E55)</f>
+        <v>29.5980789900699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subo time series con otras variables
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="h1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="h2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="h3" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="xdata1" vbProcedure="false">ROW(OFFSET(#ref!,0,0,513,1))-19*INT((-1/2+ROW(OFFSET(#ref!,0,0,513,1)))/19)</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="20">
   <si>
     <t>Site</t>
   </si>
@@ -70,6 +72,36 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>b-Sitosterol</t>
+  </si>
+  <si>
+    <t>Cholesterol</t>
+  </si>
+  <si>
+    <t>fecales</t>
+  </si>
+  <si>
+    <t>fitosteroles</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Cop/Epi</t>
+  </si>
+  <si>
+    <t>Fec/Phyto</t>
+  </si>
+  <si>
+    <t>Cop/eCop</t>
+  </si>
+  <si>
+    <t>Sito/eCop</t>
+  </si>
+  <si>
+    <t>Chnol/Chrol</t>
   </si>
 </sst>
 </file>
@@ -157,12 +189,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -201,8 +237,8 @@
   </sheetPr>
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -234,7 +270,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -254,7 +290,7 @@
       <c r="E2" s="1" t="n">
         <v>6958.72431890816</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>38642</v>
       </c>
     </row>
@@ -265,7 +301,7 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="5" t="n">
         <v>56</v>
       </c>
       <c r="D3" s="1" t="n">
@@ -274,7 +310,7 @@
       <c r="E3" s="1" t="n">
         <v>12054.6817447</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>38706</v>
       </c>
     </row>
@@ -294,7 +330,7 @@
       <c r="E4" s="1" t="n">
         <v>955.51743541604</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>38770</v>
       </c>
     </row>
@@ -314,7 +350,7 @@
       <c r="E5" s="1" t="n">
         <v>1140.17911605278</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>38864</v>
       </c>
     </row>
@@ -334,7 +370,7 @@
       <c r="E6" s="1" t="n">
         <v>1128.57105107797</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>38990</v>
       </c>
     </row>
@@ -354,7 +390,7 @@
       <c r="E7" s="1" t="n">
         <v>5124.45389911002</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>39128</v>
       </c>
     </row>
@@ -374,7 +410,7 @@
       <c r="E8" s="1" t="n">
         <v>993.275148730297</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <v>39217</v>
       </c>
     </row>
@@ -394,7 +430,7 @@
       <c r="E9" s="1" t="n">
         <v>598.101463201372</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <v>39296</v>
       </c>
     </row>
@@ -414,7 +450,7 @@
       <c r="E10" s="1" t="n">
         <v>1541.50293083238</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <v>39662</v>
       </c>
     </row>
@@ -434,7 +470,7 @@
       <c r="E11" s="1" t="n">
         <v>3135.79394610157</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <v>39775</v>
       </c>
     </row>
@@ -454,7 +490,7 @@
       <c r="E12" s="1" t="n">
         <v>2205.37322034629</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="4" t="n">
         <v>40026</v>
       </c>
     </row>
@@ -474,7 +510,7 @@
       <c r="E13" s="1" t="n">
         <v>26259.7248964433</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="4" t="n">
         <v>40238</v>
       </c>
     </row>
@@ -494,7 +530,7 @@
       <c r="E14" s="1" t="n">
         <v>28191.585503083</v>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="4" t="n">
         <v>40309</v>
       </c>
     </row>
@@ -514,7 +550,7 @@
       <c r="E15" s="1" t="n">
         <v>3814.383</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" s="4" t="n">
         <v>40392</v>
       </c>
     </row>
@@ -534,7 +570,7 @@
       <c r="E16" s="1" t="n">
         <v>5400.0357</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="4" t="n">
         <v>40464</v>
       </c>
     </row>
@@ -554,7 +590,7 @@
       <c r="E17" s="1" t="n">
         <v>5000.1016</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="4" t="n">
         <v>40695</v>
       </c>
     </row>
@@ -574,7 +610,7 @@
       <c r="E18" s="1" t="n">
         <v>24218.127503994</v>
       </c>
-      <c r="F18" s="3" t="n">
+      <c r="F18" s="4" t="n">
         <v>40954</v>
       </c>
     </row>
@@ -594,7 +630,7 @@
       <c r="E19" s="1" t="n">
         <v>3546.16830901934</v>
       </c>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="4" t="n">
         <v>41085</v>
       </c>
     </row>
@@ -614,7 +650,7 @@
       <c r="E20" s="1" t="n">
         <v>13343.2080594608</v>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="4" t="n">
         <v>41182</v>
       </c>
     </row>
@@ -634,7 +670,7 @@
       <c r="E21" s="1" t="n">
         <v>1548.33980451119</v>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="4" t="n">
         <v>41326</v>
       </c>
     </row>
@@ -654,7 +690,7 @@
       <c r="E22" s="1" t="n">
         <v>1095.46633378113</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="4" t="n">
         <v>41404</v>
       </c>
     </row>
@@ -674,7 +710,7 @@
       <c r="E23" s="1" t="n">
         <v>1585.74361309795</v>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="4" t="n">
         <v>41494</v>
       </c>
     </row>
@@ -694,7 +730,7 @@
       <c r="E24" s="1" t="n">
         <v>11428.8911784593</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="4" t="n">
         <v>41597</v>
       </c>
     </row>
@@ -714,11 +750,11 @@
       <c r="E25" s="1" t="n">
         <v>3971.84736073501</v>
       </c>
-      <c r="F25" s="3" t="n">
+      <c r="F25" s="4" t="n">
         <v>41705</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -734,11 +770,11 @@
       <c r="E26" s="1" t="n">
         <v>3.64249463</v>
       </c>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="4" t="n">
         <v>39417</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -754,11 +790,11 @@
       <c r="E27" s="1" t="n">
         <v>1.0636196</v>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="4" t="n">
         <v>39430</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -774,11 +810,11 @@
       <c r="E28" s="1" t="n">
         <v>4.16276954</v>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="4" t="n">
         <v>39465</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -794,11 +830,11 @@
       <c r="E29" s="1" t="n">
         <v>4.9376285</v>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" s="4" t="n">
         <v>39545</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -814,11 +850,11 @@
       <c r="E30" s="1" t="n">
         <v>69.962389</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="4" t="n">
         <v>39570</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
@@ -834,11 +870,11 @@
       <c r="E31" s="1" t="n">
         <v>31.7354018</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <v>39584</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -854,11 +890,11 @@
       <c r="E32" s="1" t="n">
         <v>89.3505</v>
       </c>
-      <c r="F32" s="3" t="n">
+      <c r="F32" s="4" t="n">
         <v>39661</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -874,11 +910,11 @@
       <c r="E33" s="1" t="n">
         <v>74.15866</v>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="F33" s="4" t="n">
         <v>39683</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -894,11 +930,11 @@
       <c r="E34" s="1" t="n">
         <v>68.185558876656</v>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F34" s="4" t="n">
         <v>39798</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -914,11 +950,11 @@
       <c r="E35" s="1" t="n">
         <v>17.7678461917401</v>
       </c>
-      <c r="F35" s="3" t="n">
+      <c r="F35" s="4" t="n">
         <v>39913</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -934,11 +970,11 @@
       <c r="E36" s="1" t="n">
         <v>120.560257036891</v>
       </c>
-      <c r="F36" s="3" t="n">
+      <c r="F36" s="4" t="n">
         <v>40108</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -954,11 +990,11 @@
       <c r="E37" s="1" t="n">
         <v>2.95156203066362</v>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" s="4" t="n">
         <v>40351</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -974,11 +1010,11 @@
       <c r="E38" s="1" t="n">
         <v>210.109047509172</v>
       </c>
-      <c r="F38" s="3" t="n">
+      <c r="F38" s="4" t="n">
         <v>40586</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -994,11 +1030,11 @@
       <c r="E39" s="1" t="n">
         <v>28.476289767863</v>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="4" t="n">
         <v>40748</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
@@ -1014,11 +1050,11 @@
       <c r="E40" s="1" t="n">
         <v>36.8192772320191</v>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="4" t="n">
         <v>40831</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
@@ -1034,11 +1070,11 @@
       <c r="E41" s="1" t="n">
         <v>43.4419257675166</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="4" t="n">
         <v>40922</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -1054,11 +1090,11 @@
       <c r="E42" s="1" t="n">
         <v>11.1520119651646</v>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <v>40960</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
@@ -1074,11 +1110,11 @@
       <c r="E43" s="1" t="n">
         <v>42.990298238337</v>
       </c>
-      <c r="F43" s="3" t="n">
+      <c r="F43" s="4" t="n">
         <v>41048</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -1094,11 +1130,11 @@
       <c r="E44" s="1" t="n">
         <v>25.8916144346342</v>
       </c>
-      <c r="F44" s="3" t="n">
+      <c r="F44" s="4" t="n">
         <v>41113</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
@@ -1114,11 +1150,11 @@
       <c r="E45" s="1" t="n">
         <v>4.53157722839748</v>
       </c>
-      <c r="F45" s="3" t="n">
+      <c r="F45" s="4" t="n">
         <v>41149</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -1134,11 +1170,11 @@
       <c r="E46" s="1" t="n">
         <v>15.8697727583269</v>
       </c>
-      <c r="F46" s="3" t="n">
+      <c r="F46" s="4" t="n">
         <v>41345</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -1154,11 +1190,11 @@
       <c r="E47" s="1" t="n">
         <v>13.0899746063117</v>
       </c>
-      <c r="F47" s="3" t="n">
+      <c r="F47" s="4" t="n">
         <v>41434</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
@@ -1174,11 +1210,11 @@
       <c r="E48" s="1" t="n">
         <v>4.98551502436644</v>
       </c>
-      <c r="F48" s="3" t="n">
+      <c r="F48" s="4" t="n">
         <v>41557</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
@@ -1194,11 +1230,11 @@
       <c r="E49" s="1" t="n">
         <v>56.8072268832064</v>
       </c>
-      <c r="F49" s="3" t="n">
+      <c r="F49" s="4" t="n">
         <v>41601</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
@@ -1214,11 +1250,11 @@
       <c r="E50" s="1" t="n">
         <v>31.0155893805796</v>
       </c>
-      <c r="F50" s="3" t="n">
+      <c r="F50" s="4" t="n">
         <v>41745</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
@@ -1234,11 +1270,11 @@
       <c r="E51" s="1" t="n">
         <v>111.940991000705</v>
       </c>
-      <c r="F51" s="3" t="n">
+      <c r="F51" s="4" t="n">
         <v>41955</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1254,11 +1290,11 @@
       <c r="E52" s="1" t="n">
         <v>50.6697529734385</v>
       </c>
-      <c r="F52" s="3" t="n">
+      <c r="F52" s="4" t="n">
         <v>42020</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
@@ -1274,11 +1310,11 @@
       <c r="E53" s="1" t="n">
         <v>9.99817275910024</v>
       </c>
-      <c r="F53" s="3" t="n">
+      <c r="F53" s="4" t="n">
         <v>42073</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
@@ -1294,11 +1330,11 @@
       <c r="E54" s="1" t="n">
         <v>13.5049415751479</v>
       </c>
-      <c r="F54" s="3" t="n">
+      <c r="F54" s="4" t="n">
         <v>42123</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>9</v>
       </c>
@@ -1314,11 +1350,11 @@
       <c r="E55" s="1" t="n">
         <v>74.756354115002</v>
       </c>
-      <c r="F55" s="3" t="n">
+      <c r="F55" s="4" t="n">
         <v>42134</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>9</v>
       </c>
@@ -1334,11 +1370,11 @@
       <c r="E56" s="1" t="n">
         <v>8.79824446489931</v>
       </c>
-      <c r="F56" s="3" t="n">
+      <c r="F56" s="4" t="n">
         <v>42178</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>9</v>
       </c>
@@ -1354,11 +1390,11 @@
       <c r="E57" s="1" t="n">
         <v>4.14160519354181</v>
       </c>
-      <c r="F57" s="3" t="n">
+      <c r="F57" s="4" t="n">
         <v>42210</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>9</v>
       </c>
@@ -1374,7 +1410,7 @@
       <c r="E58" s="1" t="n">
         <v>14.0865007787346</v>
       </c>
-      <c r="F58" s="3" t="n">
+      <c r="F58" s="4" t="n">
         <v>42316</v>
       </c>
     </row>
@@ -1647,15 +1683,15 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
       <c r="B15" s="0"/>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="6" t="n">
         <f aca="false">AVERAGE(C2:C14)</f>
         <v>115.481559536354</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="6" t="n">
         <f aca="false">AVERAGE(D2:D14)</f>
         <v>5577.06988194133</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="6" t="n">
         <f aca="false">AVERAGE(E2:E14)</f>
         <v>8886.76283837826</v>
       </c>
@@ -1663,15 +1699,15 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="0"/>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="6" t="n">
         <f aca="false">STDEV(C2:C14)</f>
-        <v>81.3716483219259</v>
-      </c>
-      <c r="D16" s="5" t="n">
+        <v>81.371648321926</v>
+      </c>
+      <c r="D16" s="6" t="n">
         <f aca="false">STDEV(D2:D14)</f>
         <v>5762.57295698614</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="6" t="n">
         <f aca="false">STDEV(E2:E14)</f>
         <v>8353.81566778244</v>
       </c>
@@ -1866,15 +1902,15 @@
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="0"/>
-      <c r="C28" s="5" t="n">
+      <c r="C28" s="6" t="n">
         <f aca="false">AVERAGE(C17:C27)</f>
         <v>58.6774595267746</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="D28" s="6" t="n">
         <f aca="false">AVERAGE(D17:D27)</f>
         <v>1495.62329470167</v>
       </c>
-      <c r="E28" s="5" t="n">
+      <c r="E28" s="6" t="n">
         <f aca="false">AVERAGE(E17:E27)</f>
         <v>4519.26183983132</v>
       </c>
@@ -1882,15 +1918,15 @@
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="0"/>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="6" t="n">
         <f aca="false">STDEV(C17:C27)</f>
         <v>28.9366306455723</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" s="6" t="n">
         <f aca="false">STDEV(D17:D27)</f>
         <v>1731.20460251918</v>
       </c>
-      <c r="E29" s="5" t="n">
+      <c r="E29" s="6" t="n">
         <f aca="false">STDEV(E17:E27)</f>
         <v>7973.88985444243</v>
       </c>
@@ -2187,15 +2223,15 @@
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="0"/>
-      <c r="C47" s="5" t="n">
+      <c r="C47" s="6" t="n">
         <f aca="false">AVERAGE(C30:C46)</f>
         <v>5.58827262940735</v>
       </c>
-      <c r="D47" s="5" t="n">
+      <c r="D47" s="6" t="n">
         <f aca="false">AVERAGE(D30:D46)</f>
         <v>0.419023597111637</v>
       </c>
-      <c r="E47" s="5" t="n">
+      <c r="E47" s="6" t="n">
         <f aca="false">AVERAGE(E30:E46)</f>
         <v>45.2019131079587</v>
       </c>
@@ -2203,15 +2239,15 @@
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="0"/>
-      <c r="C48" s="5" t="n">
+      <c r="C48" s="6" t="n">
         <f aca="false">STDEV(C30:C46)</f>
-        <v>3.79065528391683</v>
-      </c>
-      <c r="D48" s="5" t="n">
+        <v>3.79065528391682</v>
+      </c>
+      <c r="D48" s="6" t="n">
         <f aca="false">STDEV(D30:D46)</f>
         <v>0.503303882289127</v>
       </c>
-      <c r="E48" s="5" t="n">
+      <c r="E48" s="6" t="n">
         <f aca="false">STDEV(E30:E46)</f>
         <v>56.4130644466126</v>
       </c>
@@ -2489,29 +2525,29 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="5" t="n">
+      <c r="C65" s="6" t="n">
         <f aca="false">AVERAGE(C49:C64)</f>
         <v>3.26716432900192</v>
       </c>
-      <c r="D65" s="5" t="n">
+      <c r="D65" s="6" t="n">
         <f aca="false">AVERAGE(D49:D64)</f>
         <v>0.288032215407937</v>
       </c>
-      <c r="E65" s="5" t="n">
+      <c r="E65" s="6" t="n">
         <f aca="false">AVERAGE(E49:E64)</f>
         <v>33.3201780016949</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="5" t="n">
+      <c r="C66" s="6" t="n">
         <f aca="false">STDEV(C49:C64)</f>
-        <v>1.94453312403053</v>
-      </c>
-      <c r="D66" s="5" t="n">
+        <v>1.94453312403052</v>
+      </c>
+      <c r="D66" s="6" t="n">
         <f aca="false">STDEV(D49:D64)</f>
         <v>0.199454374093249</v>
       </c>
-      <c r="E66" s="5" t="n">
+      <c r="E66" s="6" t="n">
         <f aca="false">STDEV(E49:E64)</f>
         <v>28.6290039962637</v>
       </c>
@@ -2525,4 +2561,3078 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="7.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1001" min="7" style="1" width="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>36.5205479452055</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>262.023580350029</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>598.101463201372</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>39296</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>56.9315068493151</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>757.218821029116</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>1541.50293083238</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>39662</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>99.3150684931507</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1556.89220548716</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>3135.79394610157</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>39775</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>72.7671232876712</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>880.100578811176</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>2205.37322034629</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>40026</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>169.369863013699</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>17974.58421</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>26259.7248964433</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>37.2602739726027</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>6044.533779375</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>28191.585503083</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>40309</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>48.6575342465754</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1584.2623</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>3814.383</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>40392</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>70.4657534246575</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3488</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>5400.0357</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>40464</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>95.8082191780822</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3215</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>5000.1016</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>40695</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>146.684931506849</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>16245.12466</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>24218.127503994</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>40954</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>40.054794520548</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1625.71522722212</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>3546.16830901934</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>41085</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>131.205479452055</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>8814.324868</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>13343.2080594608</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>41182</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>101.452054794521</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>721.60910174267</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1548.33980451119</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>41326</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>51.041095890411</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>501.944855434545</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>1095.46633378113</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>41404</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>121.369863013699</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>676.517085270375</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1585.74361309795</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>41494</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>311.095890410959</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>5306.30631157449</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>11428.8911784593</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>41597</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>225.123287671233</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2395.13933587074</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>3971.84736073501</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>41705</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>3.53858734272796</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0.00841563</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>3.64249463</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>39417</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>3.42039888198792</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0.0126416</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>1.0636196</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>39430</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0.493380323584876</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>4.16276954</v>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>39465</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>7.06038611260178</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>4.9376285</v>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>39545</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>3.38245179627073</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>69.962389</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>39570</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0.345775482077364</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0.13845</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>31.7354018</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>39584</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>6.36423889360699</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>0.7545</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>89.3505</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <v>39661</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>5.11469419688291</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>74.15866</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <v>39683</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>7.86301369863014</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1.66351515740336</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>68.185558876656</v>
+      </c>
+      <c r="F27" s="4" t="n">
+        <v>39798</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1.86301369863014</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>17.7678461917401</v>
+      </c>
+      <c r="F28" s="4" t="n">
+        <v>39913</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>6.24657534246575</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>120.560257036891</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <v>40108</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>1.34246575342466</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>0.0174651905815287</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>2.95156203066362</v>
+      </c>
+      <c r="F30" s="4" t="n">
+        <v>40351</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>7.53424657534247</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>210.109047509172</v>
+      </c>
+      <c r="F31" s="4" t="n">
+        <v>40586</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>6.02739726027397</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>28.476289767863</v>
+      </c>
+      <c r="F32" s="4" t="n">
+        <v>40748</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>7.58904109589041</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0.2057</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>36.8192772320191</v>
+      </c>
+      <c r="F33" s="4" t="n">
+        <v>40831</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>9.27611175354943</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>0.7451</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>43.4419257675166</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>40922</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>2.93150684931507</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0.256290070804651</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>11.1520119651646</v>
+      </c>
+      <c r="F35" s="4" t="n">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>3.54513682453352</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>0.157966917009894</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>42.990298238337</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <v>41048</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>2.57275143492026</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>0.342678276399</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>25.8916144346342</v>
+      </c>
+      <c r="F37" s="4" t="n">
+        <v>41113</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>2.68493150684931</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>0.268100569298955</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>4.53157722839748</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>41149</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>1.78082191780822</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>0.274838168122783</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>15.8697727583269</v>
+      </c>
+      <c r="F39" s="4" t="n">
+        <v>41345</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>1.75746122477666</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>0.0331384376767369</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>13.0899746063117</v>
+      </c>
+      <c r="F40" s="4" t="n">
+        <v>41434</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>2.57534246575342</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0.126445268943807</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>4.98551502436644</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <v>41557</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>16.8284070627646</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>0.535322032720861</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>56.8072268832064</v>
+      </c>
+      <c r="F42" s="4" t="n">
+        <v>41601</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>3.12328767123288</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>0.415990409340632</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>31.0155893805796</v>
+      </c>
+      <c r="F43" s="4" t="n">
+        <v>41745</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P43"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="7.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="15" min="7" style="1" width="7"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="12.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1011" min="17" style="1" width="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>36.5205479452055</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>262.023580350029</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>598.101463201372</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>23.3299510528226</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>52.4719203756411</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>458.694758488781</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>56.5656954825621</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>30.3690888543873</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0.679340716895299</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>0.890219218170956</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>0.842405049375071</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>0.322465636387876</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>0.120119874659063</v>
+      </c>
+      <c r="P2" s="4" t="n">
+        <v>39296</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>56.9315068493151</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>757.218821029116</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>1541.50293083238</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>81.3658759590688</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>199.750773612763</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>1088.58768555181</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>165.213226260581</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>87.951245407222</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0.852070343489951</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>0.868230095620395</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>0.91395935879758</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>0.53301938457848</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>0.194084128817123</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>39662</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>99.3150684931507</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1556.89220548716</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>3135.79394610157</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>186.650936318302</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>487.682492969054</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>2163.80071985311</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>357.007701093676</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>127.303032185736</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.911780533365111</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0.858375710693799</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0.835732561154874</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0.378859029254379</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>0.102828370542711</v>
+      </c>
+      <c r="P4" s="4" t="n">
+        <v>39775</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>72.7671232876712</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>880.100578811176</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>2205.37322034629</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>120.905371124282</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>268.452108668749</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>1539.91284865858</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>251.091486445883</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>145.916776573078</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0.715372878421043</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>0.859804087838102</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>0.829805412265864</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>0.40112514355766</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>0.251079566344999</v>
+      </c>
+      <c r="P5" s="4" t="n">
+        <v>40026</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>169.369863013699</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>17974.58421</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>26259.7248964433</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>600.364975</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>3724.734223</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>20049.0182729433</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>919.470513</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>1574.5560205</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0.992329294553105</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>0.956149891277983</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>0.947351489497517</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>0.375394201366288</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>0.184476124542524</v>
+      </c>
+      <c r="P6" s="4" t="n">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>37.2602739726027</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>6044.533779375</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>28191.585503083</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1247.1291</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>6255.941672</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>18141.325055083</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>2069.380352</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>2724.938424</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>0.50242913991019</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>0.897609691976671</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>0.580635834244413</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>0.222194033047654</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>0.137818086914743</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>40309</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>48.6575342465754</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1584.2623</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>3814.383</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>201.61</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>522.1717</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>2808.6923</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>379.759</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>106.96</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>0.644335869050331</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>0.880895467965906</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>0.914224823869182</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>0.575617416131335</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>0.0954803264969858</v>
+      </c>
+      <c r="P8" s="4" t="n">
+        <v>40392</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>70.4657534246575</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3488</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>5400.0357</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>308.44</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>701.1</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>4065.4851</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>514.8306</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>118.62</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>0.91293127365429</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>0.88759931984601</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>0.944705708598212</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>0.601722490129149</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>0.107742822235797</v>
+      </c>
+      <c r="P9" s="4" t="n">
+        <v>40464</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>95.8082191780822</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3215</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>5000.1016</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>174.485</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>602.51</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>3910.2695</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>340.8471</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>146.475</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>0.908574513001235</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>0.910751714352002</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>0.356429353510263</v>
+      </c>
+      <c r="O10" s="1" t="n">
+        <v>0.130570927640171</v>
+      </c>
+      <c r="P10" s="4" t="n">
+        <v>40695</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>146.684931506849</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>16245.12466</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>24218.127503994</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>453.975221</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>2688.913766</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>19705.853907994</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>774.845158</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>1048.514672</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>0.970026190707149</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>0.962167055162363</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>0.88536652832912</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>0.177519600390078</v>
+      </c>
+      <c r="O11" s="1" t="n">
+        <v>0.154682452394081</v>
+      </c>
+      <c r="P11" s="4" t="n">
+        <v>40954</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>40.054794520548</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1625.71522722212</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>3546.16830901934</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>170.377699740651</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>455.5406527563</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>2599.02477959767</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>349.43773379893</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>142.165142866439</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>0.710219050875862</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>0.881484762919241</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>0.895950170509708</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>0.474354894147589</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>0.105969431921075</v>
+      </c>
+      <c r="P12" s="4" t="n">
+        <v>41085</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>131.205479452055</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>8814.324868</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>13343.2080594608</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>263.3207325</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1362.692777</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>10989.9898524608</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>406.5322915</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>583.9931385</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>0.970308558121483</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>0.964328390155814</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0.854667500723399</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>0.149430794154377</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>0.133918707352373</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>41182</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>101.452054794521</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>721.60910174267</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1548.33980451119</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>117.414617849922</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>210.711045368023</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>1005.89595855953</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>233.429594980964</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>98.3032056026745</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>0.930491954398859</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>0.811647880321595</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>0.830144775822125</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>0.442969640791297</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>0.101614960874043</v>
+      </c>
+      <c r="P14" s="4" t="n">
+        <v>41326</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>51.041095890411</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>501.944855434545</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>1095.46633378113</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>68.4877401544876</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>140.280005663345</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>781.865091212949</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>128.7829195595</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>44.5383173453321</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>0.782778360007331</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>0.858581012601937</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>0.845027845210065</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>0.426606203958019</v>
+      </c>
+      <c r="O15" s="1" t="n">
+        <v>0.116852697592075</v>
+      </c>
+      <c r="P15" s="4" t="n">
+        <v>41404</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>121.369863013699</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>676.517085270375</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1585.74361309795</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>30.4613655954015</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>84.2362992880512</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>1354.85874906955</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>75.1555229326906</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>86.4930418076547</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>0.963480268512876</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>0.94744421478573</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>0.638321475717996</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>0.0736169678784646</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>0.151154366976743</v>
+      </c>
+      <c r="P16" s="4" t="n">
+        <v>41494</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>311.095890410959</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>5306.30631157449</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>11428.8911784593</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>849.382640939476</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>2249.67460588636</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>7749.45654497952</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>1103.97553372725</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>726.114493866186</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>0.980990940795107</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>0.875305359106735</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0.796309175611762</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>0.384910431096598</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>0.15096193287711</v>
+      </c>
+      <c r="P17" s="4" t="n">
+        <v>41597</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>225.123287671233</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2395.13933587074</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>3971.84736073501</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>53.6972031435293</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>316.324757343522</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>3331.75735605985</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>134.129982170518</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>239.635265161118</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>0.980771862498377</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v>0.961299958977027</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>0.805825973619729</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>0.0851206323557889</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>0.136490911404911</v>
+      </c>
+      <c r="P18" s="4" t="n">
+        <v>41705</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>3.53858734272796</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0.00841563</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>3.64249463</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>0.894</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>0.932</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>0.13867363</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>2.4884</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>0.083421</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>0.450669205719509</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <v>0.0527863507198312</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>0.0655343122951622</v>
+      </c>
+      <c r="N19" s="1" t="n">
+        <v>0.881656804733728</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <v>0.0462155634696467</v>
+      </c>
+      <c r="P19" s="4" t="n">
+        <v>39417</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>3.42039888198792</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0.0126416</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>1.0636196</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>0.284545</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>0.0392746</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>0.67979</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>0.06001</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>0.490049076234853</v>
+      </c>
+      <c r="L20" s="1" t="n">
+        <v>0.0546190147588965</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>0.483989035054136</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <v>0.936864688633021</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <v>0.111227374240602</v>
+      </c>
+      <c r="P20" s="4" t="n">
+        <v>39430</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0.493380323584876</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>4.16276954</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1.064644</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>1.12546354</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>0.054314</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>2.912598</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>0.105848</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>0.397990474326352</v>
+      </c>
+      <c r="L21" s="1" t="n">
+        <v>0.0183065759955132</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>0.34021193530396</v>
+      </c>
+      <c r="N21" s="1" t="n">
+        <v>0.97825975095194</v>
+      </c>
+      <c r="O21" s="1" t="n">
+        <v>0.0470278014577331</v>
+      </c>
+      <c r="P21" s="4" t="n">
+        <v>39465</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>7.06038611260178</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>4.9376285</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>1.11455</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>1.348484</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>0.0397445</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>3.14369</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>0.40571</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>0.390969251229791</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <v>0.0124847864782517</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <v>0.588235294117647</v>
+      </c>
+      <c r="N22" s="1" t="n">
+        <v>0.99239597895093</v>
+      </c>
+      <c r="O22" s="1" t="n">
+        <v>0.0761872008790884</v>
+      </c>
+      <c r="P22" s="4" t="n">
+        <v>39545</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>3.38245179627073</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>69.962389</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>16.326</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>17.264</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>2.023454</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>47.869435</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>2.9155</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>0.379958246346555</v>
+      </c>
+      <c r="L23" s="1" t="n">
+        <v>0.0405559597881774</v>
+      </c>
+      <c r="M23" s="1" t="n">
+        <v>0.254642681751214</v>
+      </c>
+      <c r="N23" s="1" t="n">
+        <v>0.938736922168785</v>
+      </c>
+      <c r="O23" s="1" t="n">
+        <v>0.0426971276477764</v>
+      </c>
+      <c r="P23" s="4" t="n">
+        <v>39570</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0.345775482077364</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0.13845</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>31.7354018</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>8.264</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>7.236</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>1.016919</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>22.690228</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>0.8044948</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>0.346121538784612</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>0.042895039204844</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>0.202456679096293</v>
+      </c>
+      <c r="N24" s="1" t="n">
+        <v>0.938088859627216</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>0.040674550564777</v>
+      </c>
+      <c r="P24" s="4" t="n">
+        <v>39584</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>6.36423889360699</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>0.7545</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>89.3505</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>25.45</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>3.7445</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>55.996</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>0.471709909346671</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <v>0.06267942183276</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>0.386032233307751</v>
+      </c>
+      <c r="N25" s="1" t="n">
+        <v>0.956363636363636</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>0.00857031554343592</v>
+      </c>
+      <c r="P25" s="4" t="n">
+        <v>39661</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>5.11469419688291</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>74.15866</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>19.521</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>31.215</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>1.3056</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>40.5775</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>1.06056</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>0.530240265120133</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <v>0.031172477681929</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v>0.60093896713615</v>
+      </c>
+      <c r="N26" s="1" t="n">
+        <v>0.982881023110619</v>
+      </c>
+      <c r="O26" s="1" t="n">
+        <v>0.00778766687857597</v>
+      </c>
+      <c r="P26" s="4" t="n">
+        <v>39683</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>7.86301369863014</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1.66351515740336</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>68.185558876656</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>9.66170125787665</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>22.306671918434</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>12.6562636894739</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>31.8640825408869</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <v>1.3585407278612</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>0.443899270677244</v>
+      </c>
+      <c r="L27" s="1" t="n">
+        <v>0.284280441665633</v>
+      </c>
+      <c r="M27" s="1" t="n">
+        <v>0.527285843338504</v>
+      </c>
+      <c r="N27" s="1" t="n">
+        <v>0.866283314193847</v>
+      </c>
+      <c r="O27" s="1" t="n">
+        <v>0.00932642269517978</v>
+      </c>
+      <c r="P27" s="4" t="n">
+        <v>39798</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1.86301369863014</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>17.7678461917401</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>2.04365164584065</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>3.91942732040575</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>1.2251</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>8.40202846847883</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>4.72147143598277</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>0.391804750632601</v>
+      </c>
+      <c r="L28" s="1" t="n">
+        <v>0.12725497577094</v>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>0.339</v>
+      </c>
+      <c r="N28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <v>0.134409137474398</v>
+      </c>
+      <c r="P28" s="4" t="n">
+        <v>39913</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>6.24657534246575</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>120.560257036891</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>32.6581314718705</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>33.9322330097382</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>4.51149054574858</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>78.7228942223085</v>
+      </c>
+      <c r="J29" s="1" t="n">
+        <v>3.39363925909606</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>0.555555555555555</v>
+      </c>
+      <c r="L29" s="1" t="n">
+        <v>0.0542022453619428</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>0.452968226627057</v>
+      </c>
+      <c r="N29" s="1" t="n">
+        <v>0.947446753410216</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <v>0.00629626417867256</v>
+      </c>
+      <c r="P29" s="4" t="n">
+        <v>40108</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>1.34246575342466</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>0.0174651905815287</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>2.95156203066362</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0.36779706614328</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>0.274642468108201</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>0.0736394796614827</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>2.60328008289394</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>0.335835526920115</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <v>0.0275090371378905</v>
+      </c>
+      <c r="M30" s="1" t="n">
+        <v>0.446686010472253</v>
+      </c>
+      <c r="N30" s="1" t="n">
+        <v>0.944446463311737</v>
+      </c>
+      <c r="O30" s="1" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="P30" s="4" t="n">
+        <v>40351</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>7.53424657534247</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>210.109047509172</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>41.0454018504343</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>101.464573442016</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>6.0543880457329</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>76.0376842307637</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>26.5524017906589</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>0.38591404068467</v>
+      </c>
+      <c r="L31" s="1" t="n">
+        <v>0.0737511903139799</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <v>0.420289855072464</v>
+      </c>
+      <c r="N31" s="1" t="n">
+        <v>0.971594541714895</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <v>0.00177087663319953</v>
+      </c>
+      <c r="P31" s="4" t="n">
+        <v>40586</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>6.02739726027397</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>28.476289767863</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>6.79126045149589</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>6.74248880109696</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>1.52994358425678</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>74.8488318594667</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>1.49164941764262</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>0.318181818181818</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <v>0.0755820635244195</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>0.448750405881629</v>
+      </c>
+      <c r="N32" s="1" t="n">
+        <v>0.940460956077671</v>
+      </c>
+      <c r="O32" s="1" t="n">
+        <v>0.108776474371608</v>
+      </c>
+      <c r="P32" s="4" t="n">
+        <v>40748</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>7.58904109589041</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0.2057</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>36.8192772320191</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>6.12173483533562</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>11.6362918170846</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>0.466764368318796</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>23.035123056154</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v>1.68109799046179</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>0.502688172043011</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v>0.0198607184133113</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>0.945360214624125</v>
+      </c>
+      <c r="N33" s="1" t="n">
+        <v>0.998061665096232</v>
+      </c>
+      <c r="O33" s="1" t="n">
+        <v>0.0743100475278483</v>
+      </c>
+      <c r="P33" s="4" t="n">
+        <v>40831</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>9.27611175354943</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>0.7451</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>43.4419257675166</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>8.08522778181199</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>8.79236533922203</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>3.62117491165661</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>24.248424688407</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <v>6.77996082823093</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>0.331987279598386</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>0.129932792850327</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <v>0.351145601766686</v>
+      </c>
+      <c r="N34" s="1" t="n">
+        <v>0.854491011366409</v>
+      </c>
+      <c r="O34" s="1" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="P34" s="4" t="n">
+        <v>40922</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>2.93150684931507</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0.256290070804651</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>11.1520119651646</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0.943447370780038</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>2.34940942140831</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>1.45383055263918</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>3.81259605979542</v>
+      </c>
+      <c r="J35" s="1" t="n">
+        <v>3.5909039313217</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>0.801925964884528</v>
+      </c>
+      <c r="L35" s="1" t="n">
+        <v>0.276056358443604</v>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>0.257149858587852</v>
+      </c>
+      <c r="N35" s="1" t="n">
+        <v>0.56030386884196</v>
+      </c>
+      <c r="O35" s="1" t="n">
+        <v>0.065841298068045</v>
+      </c>
+      <c r="P35" s="4" t="n">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>3.54513682453352</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>0.157966917009894</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>42.990298238337</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>8.22385833129309</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>12.6778657426934</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>1.25999421437225</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>26.6283465194959</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <v>2.42409176177548</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>0.382954299983963</v>
+      </c>
+      <c r="L36" s="1" t="n">
+        <v>0.0451799634261528</v>
+      </c>
+      <c r="M36" s="1" t="n">
+        <v>0.240083373382614</v>
+      </c>
+      <c r="N36" s="1" t="n">
+        <v>0.942685910177328</v>
+      </c>
+      <c r="O36" s="1" t="n">
+        <v>0.0120013724494966</v>
+      </c>
+      <c r="P36" s="4" t="n">
+        <v>41048</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>2.57275143492026</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>0.342678276399</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>25.8916144346342</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>5.34543071858136</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>7.93481144812109</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>2.52883937947566</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>15.1960456950832</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <v>0.231917911954264</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>0.380487249183787</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <v>0.142671693996222</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <v>0.312324514888925</v>
+      </c>
+      <c r="N37" s="1" t="n">
+        <v>0.876308873076071</v>
+      </c>
+      <c r="O37" s="1" t="n">
+        <v>0.0283978936645115</v>
+      </c>
+      <c r="P37" s="4" t="n">
+        <v>41113</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>2.68493150684931</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>0.268100569298955</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>4.53157722839748</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>0.621894386703367</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>0.60928145440586</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>1.37820225694989</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>2.07876789607181</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>0.601786130721259</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>0.839104948168606</v>
+      </c>
+      <c r="L38" s="1" t="n">
+        <v>0.398673461425525</v>
+      </c>
+      <c r="M38" s="1" t="n">
+        <v>0.217394896842671</v>
+      </c>
+      <c r="N38" s="1" t="n">
+        <v>0.391859015583592</v>
+      </c>
+      <c r="O38" s="1" t="n">
+        <v>0.0186793997228127</v>
+      </c>
+      <c r="P38" s="4" t="n">
+        <v>41149</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>1.78082191780822</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>0.274838168122783</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>15.8697727583269</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>1.5769629328017</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>1.56392565422269</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>2.79017729260242</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>6.02024167042157</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <v>5.5289385823968</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>0.50141040388403</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <v>0.316690648232777</v>
+      </c>
+      <c r="M39" s="1" t="n">
+        <v>0.14593963822136</v>
+      </c>
+      <c r="N39" s="1" t="n">
+        <v>0.495066376067028</v>
+      </c>
+      <c r="O39" s="1" t="n">
+        <v>0.160444853214013</v>
+      </c>
+      <c r="P39" s="4" t="n">
+        <v>41345</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>1.75746122477666</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>0.0331384376767369</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>13.0899746063117</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>3.27570539315303</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>1.52323649997505</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>1.50411115379142</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>9.62245605247145</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <v>0.440170900073821</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>0.372969837424383</v>
+      </c>
+      <c r="L40" s="1" t="n">
+        <v>0.13518195917109</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <v>0.0254982777130885</v>
+      </c>
+      <c r="N40" s="1" t="n">
+        <v>0.72117133745651</v>
+      </c>
+      <c r="O40" s="1" t="n">
+        <v>0.0256944543517991</v>
+      </c>
+      <c r="P40" s="4" t="n">
+        <v>41434</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>2.57534246575342</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0.126445268943807</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>4.98551502436644</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>0.873454504979118</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>1.06920912874852</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>0.747294995172662</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>2.67413039042717</v>
+      </c>
+      <c r="J41" s="1" t="n">
+        <v>0.698713883876148</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>0.838513683638974</v>
+      </c>
+      <c r="L41" s="1" t="n">
+        <v>0.218416277121779</v>
+      </c>
+      <c r="M41" s="1" t="n">
+        <v>0.174903424293308</v>
+      </c>
+      <c r="N41" s="1" t="n">
+        <v>0.594205900463195</v>
+      </c>
+      <c r="O41" s="1" t="n">
+        <v>0.0063497826494831</v>
+      </c>
+      <c r="P41" s="4" t="n">
+        <v>41557</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>16.8284070627646</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>0.535322032720861</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>56.8072268832064</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>14.0808927901068</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>12.0264513708902</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>2.78227135756593</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>35.0186861137054</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>6.97981804104486</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>0.524390589118115</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <v>0.0736031980057768</v>
+      </c>
+      <c r="M42" s="1" t="n">
+        <v>0.368844864063612</v>
+      </c>
+      <c r="N42" s="1" t="n">
+        <v>0.938919093027415</v>
+      </c>
+      <c r="O42" s="1" t="n">
+        <v>0.0457119452848037</v>
+      </c>
+      <c r="P42" s="4" t="n">
+        <v>41601</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>3.12328767123288</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>0.415990409340632</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>31.0155893805796</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>6.53368734672804</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>3.61793576248273</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>2.19320899043755</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>22.4591796005272</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>2.80288001568757</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>0.77294712797797</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <v>0.088965374788931</v>
+      </c>
+      <c r="M43" s="1" t="n">
+        <v>0.211600096374653</v>
+      </c>
+      <c r="N43" s="1" t="n">
+        <v>0.808262128799209</v>
+      </c>
+      <c r="O43" s="1" t="n">
+        <v>0.0213576439986038</v>
+      </c>
+      <c r="P43" s="4" t="n">
+        <v>41745</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figuras de relaciones con caudal
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="369" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="h1" sheetId="1" state="visible" r:id="rId2"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="21">
   <si>
     <t>Site</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Chnol/Chrol</t>
+  </si>
+  <si>
+    <t>Discharge(10^3m3/s)</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="P20:P43 G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1433,7 +1436,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G63" activeCellId="0" sqref="G63"/>
+      <selection pane="topLeft" activeCell="G63" activeCellId="1" sqref="P20:P43 G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2571,7 +2574,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="P20:P43 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3460,10 +3463,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I45" activeCellId="0" sqref="I45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P43" activeCellId="0" sqref="P20:P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3474,9 +3477,10 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="7" style="1" width="7"/>
     <col collapsed="false" hidden="false" max="15" min="12" style="1" width="8.81781376518219"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="12.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1011" min="17" style="1" width="7"/>
-    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.47773279352227"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="12.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1010" min="18" style="1" width="7"/>
+    <col collapsed="false" hidden="false" max="1025" min="1011" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3525,7 +3529,10 @@
       <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3575,7 +3582,10 @@
       <c r="O2" s="1" t="n">
         <v>0.120119874659063</v>
       </c>
-      <c r="P2" s="4" t="n">
+      <c r="P2" s="5" t="n">
+        <v>24.138</v>
+      </c>
+      <c r="Q2" s="4" t="n">
         <v>39296</v>
       </c>
     </row>
@@ -3625,7 +3635,10 @@
       <c r="O3" s="1" t="n">
         <v>0.194084128817123</v>
       </c>
-      <c r="P3" s="4" t="n">
+      <c r="P3" s="5" t="n">
+        <v>21.972</v>
+      </c>
+      <c r="Q3" s="4" t="n">
         <v>39662</v>
       </c>
     </row>
@@ -3675,7 +3688,10 @@
       <c r="O4" s="1" t="n">
         <v>0.102828370542711</v>
       </c>
-      <c r="P4" s="4" t="n">
+      <c r="P4" s="5" t="n">
+        <v>32.094</v>
+      </c>
+      <c r="Q4" s="4" t="n">
         <v>39775</v>
       </c>
     </row>
@@ -3725,7 +3741,10 @@
       <c r="O5" s="1" t="n">
         <v>0.251079566344999</v>
       </c>
-      <c r="P5" s="4" t="n">
+      <c r="P5" s="5" t="n">
+        <v>24.002</v>
+      </c>
+      <c r="Q5" s="4" t="n">
         <v>40026</v>
       </c>
     </row>
@@ -3775,7 +3794,10 @@
       <c r="O6" s="1" t="n">
         <v>0.184476124542524</v>
       </c>
-      <c r="P6" s="4" t="n">
+      <c r="P6" s="5" t="n">
+        <v>46.088</v>
+      </c>
+      <c r="Q6" s="4" t="n">
         <v>40238</v>
       </c>
     </row>
@@ -3825,7 +3847,10 @@
       <c r="O7" s="1" t="n">
         <v>0.137818086914743</v>
       </c>
-      <c r="P7" s="4" t="n">
+      <c r="P7" s="5" t="n">
+        <v>26.261</v>
+      </c>
+      <c r="Q7" s="4" t="n">
         <v>40309</v>
       </c>
     </row>
@@ -3875,7 +3900,10 @@
       <c r="O8" s="1" t="n">
         <v>0.0954803264969858</v>
       </c>
-      <c r="P8" s="4" t="n">
+      <c r="P8" s="5" t="n">
+        <v>25.655</v>
+      </c>
+      <c r="Q8" s="4" t="n">
         <v>40392</v>
       </c>
     </row>
@@ -3925,7 +3953,10 @@
       <c r="O9" s="1" t="n">
         <v>0.107742822235797</v>
       </c>
-      <c r="P9" s="4" t="n">
+      <c r="P9" s="5" t="n">
+        <v>21.687</v>
+      </c>
+      <c r="Q9" s="4" t="n">
         <v>40464</v>
       </c>
     </row>
@@ -3975,7 +4006,10 @@
       <c r="O10" s="1" t="n">
         <v>0.130570927640171</v>
       </c>
-      <c r="P10" s="4" t="n">
+      <c r="P10" s="5" t="n">
+        <v>24.077</v>
+      </c>
+      <c r="Q10" s="4" t="n">
         <v>40695</v>
       </c>
     </row>
@@ -4025,7 +4059,10 @@
       <c r="O11" s="1" t="n">
         <v>0.154682452394081</v>
       </c>
-      <c r="P11" s="4" t="n">
+      <c r="P11" s="5" t="n">
+        <v>24.184</v>
+      </c>
+      <c r="Q11" s="4" t="n">
         <v>40954</v>
       </c>
     </row>
@@ -4075,7 +4112,10 @@
       <c r="O12" s="1" t="n">
         <v>0.105969431921075</v>
       </c>
-      <c r="P12" s="4" t="n">
+      <c r="P12" s="5" t="n">
+        <v>19.465</v>
+      </c>
+      <c r="Q12" s="4" t="n">
         <v>41085</v>
       </c>
     </row>
@@ -4125,7 +4165,10 @@
       <c r="O13" s="1" t="n">
         <v>0.133918707352373</v>
       </c>
-      <c r="P13" s="4" t="n">
+      <c r="P13" s="5" t="n">
+        <v>37.927</v>
+      </c>
+      <c r="Q13" s="4" t="n">
         <v>41182</v>
       </c>
     </row>
@@ -4175,7 +4218,10 @@
       <c r="O14" s="1" t="n">
         <v>0.101614960874043</v>
       </c>
-      <c r="P14" s="4" t="n">
+      <c r="P14" s="5" t="n">
+        <v>19.973</v>
+      </c>
+      <c r="Q14" s="4" t="n">
         <v>41326</v>
       </c>
     </row>
@@ -4225,7 +4271,10 @@
       <c r="O15" s="1" t="n">
         <v>0.116852697592075</v>
       </c>
-      <c r="P15" s="4" t="n">
+      <c r="P15" s="5" t="n">
+        <v>22.676</v>
+      </c>
+      <c r="Q15" s="4" t="n">
         <v>41404</v>
       </c>
     </row>
@@ -4275,7 +4324,10 @@
       <c r="O16" s="1" t="n">
         <v>0.151154366976743</v>
       </c>
-      <c r="P16" s="4" t="n">
+      <c r="P16" s="5" t="n">
+        <v>28.29</v>
+      </c>
+      <c r="Q16" s="4" t="n">
         <v>41494</v>
       </c>
     </row>
@@ -4325,7 +4377,10 @@
       <c r="O17" s="1" t="n">
         <v>0.15096193287711</v>
       </c>
-      <c r="P17" s="4" t="n">
+      <c r="P17" s="5" t="n">
+        <v>25.099</v>
+      </c>
+      <c r="Q17" s="4" t="n">
         <v>41597</v>
       </c>
     </row>
@@ -4375,7 +4430,10 @@
       <c r="O18" s="1" t="n">
         <v>0.136490911404911</v>
       </c>
-      <c r="P18" s="4" t="n">
+      <c r="P18" s="5" t="n">
+        <v>27.418</v>
+      </c>
+      <c r="Q18" s="4" t="n">
         <v>41705</v>
       </c>
     </row>
@@ -4425,7 +4483,10 @@
       <c r="O19" s="1" t="n">
         <v>0.0462155634696467</v>
       </c>
-      <c r="P19" s="4" t="n">
+      <c r="P19" s="1" t="n">
+        <v>3.1943</v>
+      </c>
+      <c r="Q19" s="4" t="n">
         <v>39417</v>
       </c>
     </row>
@@ -4475,7 +4536,10 @@
       <c r="O20" s="1" t="n">
         <v>0.111227374240602</v>
       </c>
-      <c r="P20" s="4" t="n">
+      <c r="P20" s="1" t="n">
+        <v>3.03455555555556</v>
+      </c>
+      <c r="Q20" s="4" t="n">
         <v>39430</v>
       </c>
     </row>
@@ -4525,7 +4589,10 @@
       <c r="O21" s="1" t="n">
         <v>0.0470278014577331</v>
       </c>
-      <c r="P21" s="4" t="n">
+      <c r="P21" s="1" t="n">
+        <v>1.84434920634921</v>
+      </c>
+      <c r="Q21" s="4" t="n">
         <v>39465</v>
       </c>
     </row>
@@ -4575,7 +4642,10 @@
       <c r="O22" s="1" t="n">
         <v>0.0761872008790884</v>
       </c>
-      <c r="P22" s="4" t="n">
+      <c r="P22" s="1" t="n">
+        <v>0.4198</v>
+      </c>
+      <c r="Q22" s="4" t="n">
         <v>39545</v>
       </c>
     </row>
@@ -4625,7 +4695,10 @@
       <c r="O23" s="1" t="n">
         <v>0.0426971276477764</v>
       </c>
-      <c r="P23" s="4" t="n">
+      <c r="P23" s="1" t="n">
+        <v>3.6076</v>
+      </c>
+      <c r="Q23" s="4" t="n">
         <v>39570</v>
       </c>
     </row>
@@ -4675,7 +4748,10 @@
       <c r="O24" s="1" t="n">
         <v>0.040674550564777</v>
       </c>
-      <c r="P24" s="4" t="n">
+      <c r="P24" s="1" t="n">
+        <v>2.45333333333333</v>
+      </c>
+      <c r="Q24" s="4" t="n">
         <v>39584</v>
       </c>
     </row>
@@ -4725,7 +4801,10 @@
       <c r="O25" s="1" t="n">
         <v>0.00857031554343592</v>
       </c>
-      <c r="P25" s="4" t="n">
+      <c r="P25" s="1" t="n">
+        <v>4.20135714285714</v>
+      </c>
+      <c r="Q25" s="4" t="n">
         <v>39661</v>
       </c>
     </row>
@@ -4775,7 +4854,10 @@
       <c r="O26" s="1" t="n">
         <v>0.00778766687857597</v>
       </c>
-      <c r="P26" s="4" t="n">
+      <c r="P26" s="1" t="n">
+        <v>4.49893103448276</v>
+      </c>
+      <c r="Q26" s="4" t="n">
         <v>39683</v>
       </c>
     </row>
@@ -4825,7 +4907,10 @@
       <c r="O27" s="1" t="n">
         <v>0.00932642269517978</v>
       </c>
-      <c r="P27" s="4" t="n">
+      <c r="P27" s="1" t="n">
+        <v>1.9989375</v>
+      </c>
+      <c r="Q27" s="4" t="n">
         <v>39798</v>
       </c>
     </row>
@@ -4875,7 +4960,10 @@
       <c r="O28" s="1" t="n">
         <v>0.134409137474398</v>
       </c>
-      <c r="P28" s="4" t="n">
+      <c r="P28" s="1" t="n">
+        <v>1.092875</v>
+      </c>
+      <c r="Q28" s="4" t="n">
         <v>39913</v>
       </c>
     </row>
@@ -4925,7 +5013,10 @@
       <c r="O29" s="1" t="n">
         <v>0.00629626417867256</v>
       </c>
-      <c r="P29" s="4" t="n">
+      <c r="P29" s="1" t="n">
+        <v>7.55820689655172</v>
+      </c>
+      <c r="Q29" s="4" t="n">
         <v>40108</v>
       </c>
     </row>
@@ -4975,7 +5066,10 @@
       <c r="O30" s="1" t="n">
         <v>0.053</v>
       </c>
-      <c r="P30" s="4" t="n">
+      <c r="P30" s="1" t="n">
+        <v>4.28184375</v>
+      </c>
+      <c r="Q30" s="4" t="n">
         <v>40351</v>
       </c>
     </row>
@@ -5025,7 +5119,10 @@
       <c r="O31" s="1" t="n">
         <v>0.00177087663319953</v>
       </c>
-      <c r="P31" s="4" t="n">
+      <c r="P31" s="1" t="n">
+        <v>4.31807692307692</v>
+      </c>
+      <c r="Q31" s="4" t="n">
         <v>40586</v>
       </c>
     </row>
@@ -5075,7 +5172,10 @@
       <c r="O32" s="1" t="n">
         <v>0.108776474371608</v>
       </c>
-      <c r="P32" s="4" t="n">
+      <c r="P32" s="1" t="n">
+        <v>8.40998620689655</v>
+      </c>
+      <c r="Q32" s="4" t="n">
         <v>40748</v>
       </c>
     </row>
@@ -5125,7 +5225,10 @@
       <c r="O33" s="1" t="n">
         <v>0.0743100475278483</v>
       </c>
-      <c r="P33" s="4" t="n">
+      <c r="P33" s="1" t="n">
+        <v>5.81072413793103</v>
+      </c>
+      <c r="Q33" s="4" t="n">
         <v>40831</v>
       </c>
     </row>
@@ -5175,7 +5278,10 @@
       <c r="O34" s="1" t="n">
         <v>0.056</v>
       </c>
-      <c r="P34" s="4" t="n">
+      <c r="P34" s="1" t="n">
+        <v>1.00637096774194</v>
+      </c>
+      <c r="Q34" s="4" t="n">
         <v>40922</v>
       </c>
     </row>
@@ -5225,7 +5331,10 @@
       <c r="O35" s="1" t="n">
         <v>0.065841298068045</v>
       </c>
-      <c r="P35" s="4" t="n">
+      <c r="P35" s="1" t="n">
+        <v>1.10518181818182</v>
+      </c>
+      <c r="Q35" s="4" t="n">
         <v>40960</v>
       </c>
     </row>
@@ -5275,7 +5384,10 @@
       <c r="O36" s="1" t="n">
         <v>0.0120013724494966</v>
       </c>
-      <c r="P36" s="4" t="n">
+      <c r="P36" s="1" t="n">
+        <v>0.72490625</v>
+      </c>
+      <c r="Q36" s="4" t="n">
         <v>41048</v>
       </c>
     </row>
@@ -5325,7 +5437,10 @@
       <c r="O37" s="1" t="n">
         <v>0.0283978936645115</v>
       </c>
-      <c r="P37" s="4" t="n">
+      <c r="P37" s="1" t="n">
+        <v>2.32294117647059</v>
+      </c>
+      <c r="Q37" s="4" t="n">
         <v>41113</v>
       </c>
     </row>
@@ -5375,7 +5490,10 @@
       <c r="O38" s="1" t="n">
         <v>0.0186793997228127</v>
       </c>
-      <c r="P38" s="4" t="n">
+      <c r="P38" s="1" t="n">
+        <v>2.98763888888889</v>
+      </c>
+      <c r="Q38" s="4" t="n">
         <v>41149</v>
       </c>
     </row>
@@ -5425,7 +5543,10 @@
       <c r="O39" s="1" t="n">
         <v>0.160444853214013</v>
       </c>
-      <c r="P39" s="4" t="n">
+      <c r="P39" s="1" t="n">
+        <v>5.59122222222222</v>
+      </c>
+      <c r="Q39" s="4" t="n">
         <v>41345</v>
       </c>
     </row>
@@ -5475,7 +5596,10 @@
       <c r="O40" s="1" t="n">
         <v>0.0256944543517991</v>
       </c>
-      <c r="P40" s="4" t="n">
+      <c r="P40" s="1" t="n">
+        <v>4.38019871794872</v>
+      </c>
+      <c r="Q40" s="4" t="n">
         <v>41434</v>
       </c>
     </row>
@@ -5525,7 +5649,10 @@
       <c r="O41" s="1" t="n">
         <v>0.0063497826494831</v>
       </c>
-      <c r="P41" s="4" t="n">
+      <c r="P41" s="1" t="n">
+        <v>4.96918181818182</v>
+      </c>
+      <c r="Q41" s="4" t="n">
         <v>41557</v>
       </c>
     </row>
@@ -5575,7 +5702,10 @@
       <c r="O42" s="1" t="n">
         <v>0.0457119452848037</v>
       </c>
-      <c r="P42" s="4" t="n">
+      <c r="P42" s="1" t="n">
+        <v>8.30087931034483</v>
+      </c>
+      <c r="Q42" s="4" t="n">
         <v>41601</v>
       </c>
     </row>
@@ -5625,8 +5755,111 @@
       <c r="O43" s="1" t="n">
         <v>0.0213576439986038</v>
       </c>
-      <c r="P43" s="4" t="n">
+      <c r="P43" s="1" t="n">
+        <v>6.4781</v>
+      </c>
+      <c r="Q43" s="4" t="n">
         <v>41745</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K44" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L44" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M44" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N44" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="O44" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="P44" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q44" s="1" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="L45" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="N45" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="O45" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="P45" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q45" s="1" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corregi la escala del flux
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="369" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="369" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="h1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="Corr_Matrix" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="h4" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="h5" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="h6" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="xdata1" vbProcedure="false">ROW(OFFSET(#ref!,0,0,513,1))-19*INT((-1/2+ROW(OFFSET(#ref!,0,0,513,1)))/19)</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="37">
   <si>
     <t>Site</t>
   </si>
@@ -2624,8 +2625,8 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3516,11 +3517,11 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N152" activeCellId="0" sqref="N152"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S9" activeCellId="0" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="7"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1417004048583"/>
@@ -3533,9 +3534,10 @@
     <col collapsed="false" hidden="false" max="15" min="12" style="1" width="8.85425101214575"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="12.1417004048583"/>
-    <col collapsed="false" hidden="false" max="970" min="18" style="1" width="7"/>
-    <col collapsed="false" hidden="false" max="987" min="971" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="1008" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="969" min="18" style="1" width="7"/>
+    <col collapsed="false" hidden="false" max="986" min="970" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1006" min="987" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="1007" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3599,7 +3601,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>36.5205479452055</v>
+        <v>11.7340520547945</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>262.023580350029</v>
@@ -3652,7 +3654,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>56.9315068493151</v>
+        <v>18.2920931506849</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>757.218821029116</v>
@@ -3705,7 +3707,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>99.3150684931507</v>
+        <v>31.9099315068493</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1556.89220548716</v>
@@ -3758,7 +3760,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>72.7671232876712</v>
+        <v>23.3800767123288</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>880.100578811176</v>
@@ -3811,7 +3813,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>169.369863013699</v>
+        <v>54.4185369863015</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>17974.58421</v>
@@ -3864,7 +3866,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>37.2602739726027</v>
+        <v>11.9717260273972</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>4044.533779375</v>
@@ -3917,7 +3919,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>48.6575342465754</v>
+        <v>15.6336657534247</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1584.2623</v>
@@ -3970,7 +3972,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>70.4657534246575</v>
+        <v>22.6406465753425</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>3488</v>
@@ -4023,7 +4025,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>95.8082191780822</v>
+        <v>30.7831808219178</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3215</v>
@@ -4076,7 +4078,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>146.684931506849</v>
+        <v>47.1298684931506</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>16245.12466</v>
@@ -4129,7 +4131,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>40.054794520548</v>
+        <v>12.8696054794521</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1625.71522722212</v>
@@ -4182,7 +4184,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>131.205479452055</v>
+        <v>42.1563205479453</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>8814.324868</v>
@@ -4235,7 +4237,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>101.452054794521</v>
+        <v>32.5965452054796</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>721.60910174267</v>
@@ -4288,7 +4290,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>51.041095890411</v>
+        <v>16.3995041095891</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>501.944855434545</v>
@@ -4341,7 +4343,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>121.369863013699</v>
+        <v>38.9961369863015</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>676.517085270375</v>
@@ -4394,7 +4396,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>311.095890410959</v>
+        <v>99.9551095890411</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>5306.30631157449</v>
@@ -4447,7 +4449,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>225.123287671233</v>
+        <v>72.3321123287672</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>2395.13933587074</v>
@@ -4500,7 +4502,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>3.53858734272796</v>
+        <v>1.13694811321849</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0.00841563</v>
@@ -4553,7 +4555,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>3.42039888198792</v>
+        <v>1.09897416078272</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0.0126416</v>
@@ -4606,7 +4608,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0.493380323584876</v>
+        <v>0.158523097967821</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>0.0122</v>
@@ -4659,7 +4661,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>7.06038611260178</v>
+        <v>2.26850205797895</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>0.0122</v>
@@ -4712,7 +4714,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>3.38245179627073</v>
+        <v>1.08678176214179</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>0.364</v>
@@ -4765,7 +4767,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>0.345775482077364</v>
+        <v>0.111097662391457</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>0.13845</v>
@@ -4818,7 +4820,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>6.36423889360699</v>
+        <v>2.04482995651593</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>0.7545</v>
@@ -4871,7 +4873,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>5.11469419688291</v>
+        <v>1.64335124545848</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>0.512</v>
@@ -4924,7 +4926,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>7.86301369863014</v>
+        <v>2.52638630136986</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>1.66351515740336</v>
@@ -4977,7 +4979,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>1.86301369863014</v>
+        <v>0.598586301369864</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>0.48</v>
@@ -5030,7 +5032,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>6.24657534246575</v>
+        <v>2.00702465753425</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>1.5</v>
@@ -5083,7 +5085,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>1.34246575342466</v>
+        <v>0.431334246575343</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>0.0174651905815287</v>
@@ -5136,7 +5138,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>7.53424657534247</v>
+        <v>2.42075342465754</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>0.87</v>
@@ -5189,7 +5191,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>6.02739726027397</v>
+        <v>1.93660273972603</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>0.35</v>
@@ -5242,7 +5244,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>7.58904109589041</v>
+        <v>2.43835890410959</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>0.2057</v>
@@ -5295,7 +5297,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>9.27611175354943</v>
+        <v>2.98041470641543</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>0.7451</v>
@@ -5348,7 +5350,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>2.93150684931507</v>
+        <v>0.941893150684932</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>0.256290070804651</v>
@@ -5401,7 +5403,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>3.54513682453352</v>
+        <v>1.13905246172262</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>0.157966917009894</v>
@@ -5454,7 +5456,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>2.57275143492026</v>
+        <v>0.82662503603988</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>0.342678276399</v>
@@ -5507,7 +5509,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>2.68493150684931</v>
+        <v>0.862668493150683</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0.268100569298955</v>
@@ -5560,7 +5562,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>1.78082191780822</v>
+        <v>0.572178082191781</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>0.274838168122783</v>
@@ -5613,7 +5615,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>1.75746122477666</v>
+        <v>0.564672291520741</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>0.0331384376767369</v>
@@ -5666,7 +5668,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>2.57534246575342</v>
+        <v>0.827457534246574</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>0.126445268943807</v>
@@ -5719,7 +5721,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>16.8284070627646</v>
+        <v>5.40696718926627</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>0.535322032720861</v>
@@ -5772,7 +5774,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>3.12328767123288</v>
+        <v>1.00351232876712</v>
       </c>
       <c r="D43" s="1" t="n">
         <v>0.415990409340632</v>
@@ -11637,7 +11639,7 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -11687,7 +11689,7 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">G2-E2-D2-C2</f>
-        <v>323.471908000002</v>
+        <v>323.471908</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>6958.72431890816</v>
@@ -12047,7 +12049,7 @@
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">G17-E17-D17-C17</f>
-        <v>-943.357100000001</v>
+        <v>-943.3571</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>5000.1016</v>
@@ -13035,6 +13037,897 @@
       </c>
       <c r="G58" s="0" t="n">
         <v>14.0865007787346</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="7.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>11.7340520547945</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>262.023580350029</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>598.101463201372</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>39296</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>18.2920931506849</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>757.218821029116</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>1541.50293083238</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>39662</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>31.9099315068493</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1556.89220548716</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>3135.79394610157</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>39775</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>23.3800767123288</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>880.100578811176</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>2205.37322034629</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>40026</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>54.4185369863015</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>17974.58421</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>26259.7248964433</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>11.9717260273972</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>4044.533779375</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>12691.585503083</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>40309</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>15.6336657534247</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1584.2623</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>3814.383</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>40392</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>22.6406465753425</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3488</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>5400.0357</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>40464</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>30.7831808219178</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3215</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>5000.1016</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>40695</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>47.1298684931506</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>16245.12466</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>24218.127503994</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>40954</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>12.8696054794521</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1625.71522722212</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>3546.16830901934</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>41085</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>42.1563205479453</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>8814.324868</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>13343.2080594608</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>41182</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>32.5965452054796</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>721.60910174267</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1548.33980451119</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>41326</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>16.3995041095891</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>501.944855434545</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>1095.46633378113</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>41404</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>38.9961369863015</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>676.517085270375</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1585.74361309795</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>41494</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>99.9551095890411</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>5306.30631157449</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>11428.8911784593</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>41597</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>72.3321123287672</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2395.13933587074</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>3971.84736073501</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>41705</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1.13694811321849</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0.00841563</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>3.64249463</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>39417</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>1.09897416078272</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0.0126416</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>1.0636196</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>39430</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0.158523097967821</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>4.16276954</v>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>39465</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>2.26850205797895</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>4.9376285</v>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>39545</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1.08678176214179</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>69.962389</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>39570</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0.111097662391457</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0.13845</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>31.7354018</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>39584</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>2.04482995651593</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>0.7545</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>89.3505</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <v>39661</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>1.64335124545848</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>74.15866</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <v>39683</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>2.52638630136986</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1.66351515740336</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>68.185558876656</v>
+      </c>
+      <c r="F27" s="4" t="n">
+        <v>39798</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>0.598586301369864</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>17.7678461917401</v>
+      </c>
+      <c r="F28" s="4" t="n">
+        <v>39913</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>2.00702465753425</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>120.560257036891</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <v>40108</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0.431334246575343</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>0.0174651905815287</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>2.95156203066362</v>
+      </c>
+      <c r="F30" s="4" t="n">
+        <v>40351</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>2.42075342465754</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>210.109047509172</v>
+      </c>
+      <c r="F31" s="4" t="n">
+        <v>40586</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1.93660273972603</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>28.476289767863</v>
+      </c>
+      <c r="F32" s="4" t="n">
+        <v>40748</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>2.43835890410959</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0.2057</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>36.8192772320191</v>
+      </c>
+      <c r="F33" s="4" t="n">
+        <v>40831</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>2.98041470641543</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>0.7451</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>43.4419257675166</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>40922</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0.941893150684932</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0.256290070804651</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>11.1520119651646</v>
+      </c>
+      <c r="F35" s="4" t="n">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>1.13905246172262</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>0.157966917009894</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>42.990298238337</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <v>41048</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>0.82662503603988</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>0.342678276399</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>25.8916144346342</v>
+      </c>
+      <c r="F37" s="4" t="n">
+        <v>41113</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>0.862668493150683</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>0.268100569298955</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>4.53157722839748</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>41149</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>0.572178082191781</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>0.274838168122783</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>15.8697727583269</v>
+      </c>
+      <c r="F39" s="4" t="n">
+        <v>41345</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>0.564672291520741</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>0.0331384376767369</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>13.0899746063117</v>
+      </c>
+      <c r="F40" s="4" t="n">
+        <v>41434</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>0.827457534246574</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0.126445268943807</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>4.98551502436644</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <v>41557</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>5.40696718926627</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>0.535322032720861</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>56.8072268832064</v>
+      </c>
+      <c r="F42" s="4" t="n">
+        <v>41601</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1.00351232876712</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>0.415990409340632</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>31.0155893805796</v>
+      </c>
+      <c r="F43" s="4" t="n">
+        <v>41745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corregi el error de flux en N
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="369" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="369" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="h1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1510,7 +1510,7 @@
   </sheetPr>
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4463,7 +4463,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6490,10 +6490,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7477,7 +7477,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>1.13694811321849</v>
+        <v>3.53858734272795</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0.00841563</v>
@@ -7521,6 +7521,7 @@
       <c r="Q19" s="4" t="n">
         <v>39417</v>
       </c>
+      <c r="R19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -7530,7 +7531,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>1.09897416078272</v>
+        <v>3.42039888198792</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0.0126416</v>
@@ -7574,6 +7575,7 @@
       <c r="Q20" s="4" t="n">
         <v>39430</v>
       </c>
+      <c r="R20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -7583,7 +7585,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0.158523097967821</v>
+        <v>0.493380323584877</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>0.0122</v>
@@ -7627,6 +7629,7 @@
       <c r="Q21" s="4" t="n">
         <v>39465</v>
       </c>
+      <c r="R21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -7636,7 +7639,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>2.26850205797895</v>
+        <v>7.06038611260177</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>0.0122</v>
@@ -7680,6 +7683,7 @@
       <c r="Q22" s="4" t="n">
         <v>39545</v>
       </c>
+      <c r="R22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -7689,7 +7693,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>1.08678176214179</v>
+        <v>3.38245179627074</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>0.364</v>
@@ -7733,6 +7737,7 @@
       <c r="Q23" s="4" t="n">
         <v>39570</v>
       </c>
+      <c r="R23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -7742,7 +7747,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>0.111097662391457</v>
+        <v>0.345775482077364</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>0.13845</v>
@@ -7786,6 +7791,7 @@
       <c r="Q24" s="4" t="n">
         <v>39584</v>
       </c>
+      <c r="R24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -7795,7 +7801,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>2.04482995651593</v>
+        <v>6.364238893607</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>0.7545</v>
@@ -7839,6 +7845,7 @@
       <c r="Q25" s="4" t="n">
         <v>39661</v>
       </c>
+      <c r="R25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -7848,7 +7855,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>1.64335124545848</v>
+        <v>5.11469419688291</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>0.512</v>
@@ -7892,6 +7899,7 @@
       <c r="Q26" s="4" t="n">
         <v>39683</v>
       </c>
+      <c r="R26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -7901,7 +7909,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>2.52638630136986</v>
+        <v>7.86301369863013</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>1.66351515740336</v>
@@ -7945,6 +7953,7 @@
       <c r="Q27" s="4" t="n">
         <v>39798</v>
       </c>
+      <c r="R27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -7954,7 +7963,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>0.598586301369864</v>
+        <v>1.86301369863014</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>0.48</v>
@@ -7998,6 +8007,7 @@
       <c r="Q28" s="4" t="n">
         <v>39913</v>
       </c>
+      <c r="R28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -8007,7 +8017,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>2.00702465753425</v>
+        <v>6.24657534246576</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>1.5</v>
@@ -8051,6 +8061,7 @@
       <c r="Q29" s="4" t="n">
         <v>40108</v>
       </c>
+      <c r="R29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -8060,7 +8071,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>0.431334246575343</v>
+        <v>1.34246575342466</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>0.0174651905815287</v>
@@ -8104,6 +8115,7 @@
       <c r="Q30" s="4" t="n">
         <v>40351</v>
       </c>
+      <c r="R30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -8113,7 +8125,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>2.42075342465754</v>
+        <v>7.53424657534248</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>0.87</v>
@@ -8157,6 +8169,7 @@
       <c r="Q31" s="4" t="n">
         <v>40586</v>
       </c>
+      <c r="R31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -8166,7 +8179,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>1.93660273972603</v>
+        <v>6.02739726027398</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>0.35</v>
@@ -8210,6 +8223,7 @@
       <c r="Q32" s="4" t="n">
         <v>40748</v>
       </c>
+      <c r="R32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -8219,7 +8233,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>2.43835890410959</v>
+        <v>7.58904109589041</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>0.2057</v>
@@ -8263,6 +8277,7 @@
       <c r="Q33" s="4" t="n">
         <v>40831</v>
       </c>
+      <c r="R33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -8272,7 +8287,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>2.98041470641543</v>
+        <v>9.27611175354942</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>0.7451</v>
@@ -8316,6 +8331,7 @@
       <c r="Q34" s="4" t="n">
         <v>40922</v>
       </c>
+      <c r="R34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -8325,7 +8341,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>0.941893150684932</v>
+        <v>2.93150684931507</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>0.256290070804651</v>
@@ -8369,6 +8385,7 @@
       <c r="Q35" s="4" t="n">
         <v>40960</v>
       </c>
+      <c r="R35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -8378,7 +8395,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>1.13905246172262</v>
+        <v>3.54513682453352</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>0.157966917009894</v>
@@ -8422,6 +8439,7 @@
       <c r="Q36" s="4" t="n">
         <v>41048</v>
       </c>
+      <c r="R36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -8431,7 +8449,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>0.82662503603988</v>
+        <v>2.57275143492026</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>0.342678276399</v>
@@ -8475,6 +8493,7 @@
       <c r="Q37" s="4" t="n">
         <v>41113</v>
       </c>
+      <c r="R37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
@@ -8484,7 +8503,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>0.862668493150683</v>
+        <v>2.68493150684931</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0.268100569298955</v>
@@ -8528,6 +8547,7 @@
       <c r="Q38" s="4" t="n">
         <v>41149</v>
       </c>
+      <c r="R38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -8537,7 +8557,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>0.572178082191781</v>
+        <v>1.78082191780822</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>0.274838168122783</v>
@@ -8581,6 +8601,7 @@
       <c r="Q39" s="4" t="n">
         <v>41345</v>
       </c>
+      <c r="R39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
@@ -8590,7 +8611,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>0.564672291520741</v>
+        <v>1.75746122477666</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>0.0331384376767369</v>
@@ -8634,6 +8655,7 @@
       <c r="Q40" s="4" t="n">
         <v>41434</v>
       </c>
+      <c r="R40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
@@ -8643,7 +8665,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>0.827457534246574</v>
+        <v>2.57534246575342</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>0.126445268943807</v>
@@ -8687,6 +8709,7 @@
       <c r="Q41" s="4" t="n">
         <v>41557</v>
       </c>
+      <c r="R41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -8696,7 +8719,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>5.40696718926627</v>
+        <v>16.8284070627646</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>0.535322032720861</v>
@@ -8740,6 +8763,7 @@
       <c r="Q42" s="4" t="n">
         <v>41601</v>
       </c>
+      <c r="R42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -8749,7 +8773,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>1.00351232876712</v>
+        <v>3.12328767123287</v>
       </c>
       <c r="D43" s="1" t="n">
         <v>0.415990409340632</v>
@@ -8793,6 +8817,7 @@
       <c r="Q43" s="4" t="n">
         <v>41745</v>
       </c>
+      <c r="R43" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
chequeo las diferencias warm cold en flux
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -6493,7 +6493,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6567,6 +6567,7 @@
       <c r="Q1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="R1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -6620,6 +6621,7 @@
       <c r="Q2" s="4" t="n">
         <v>39296</v>
       </c>
+      <c r="R2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -6673,6 +6675,7 @@
       <c r="Q3" s="4" t="n">
         <v>39662</v>
       </c>
+      <c r="R3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -6726,6 +6729,7 @@
       <c r="Q4" s="4" t="n">
         <v>39775</v>
       </c>
+      <c r="R4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -6779,6 +6783,7 @@
       <c r="Q5" s="4" t="n">
         <v>40026</v>
       </c>
+      <c r="R5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -6832,6 +6837,7 @@
       <c r="Q6" s="4" t="n">
         <v>40238</v>
       </c>
+      <c r="R6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -6885,6 +6891,7 @@
       <c r="Q7" s="4" t="n">
         <v>40309</v>
       </c>
+      <c r="R7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -6938,6 +6945,7 @@
       <c r="Q8" s="4" t="n">
         <v>40392</v>
       </c>
+      <c r="R8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -6991,6 +6999,7 @@
       <c r="Q9" s="4" t="n">
         <v>40464</v>
       </c>
+      <c r="R9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -7044,6 +7053,7 @@
       <c r="Q10" s="4" t="n">
         <v>40695</v>
       </c>
+      <c r="R10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -7097,6 +7107,7 @@
       <c r="Q11" s="4" t="n">
         <v>40954</v>
       </c>
+      <c r="R11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -7150,6 +7161,7 @@
       <c r="Q12" s="4" t="n">
         <v>41085</v>
       </c>
+      <c r="R12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -7203,6 +7215,7 @@
       <c r="Q13" s="4" t="n">
         <v>41182</v>
       </c>
+      <c r="R13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -7256,6 +7269,7 @@
       <c r="Q14" s="4" t="n">
         <v>41326</v>
       </c>
+      <c r="R14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -7309,6 +7323,7 @@
       <c r="Q15" s="4" t="n">
         <v>41404</v>
       </c>
+      <c r="R15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -7362,6 +7377,7 @@
       <c r="Q16" s="4" t="n">
         <v>41494</v>
       </c>
+      <c r="R16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -7415,6 +7431,7 @@
       <c r="Q17" s="4" t="n">
         <v>41597</v>
       </c>
+      <c r="R17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -7468,6 +7485,7 @@
       <c r="Q18" s="4" t="n">
         <v>41705</v>
       </c>
+      <c r="R18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -7585,7 +7603,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0.493380323584877</v>
+        <v>0.49338032358488</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>0.0122</v>

</xml_diff>

<commit_message>
reparo el git luego de crash inesperado
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -6492,8 +6492,8 @@
   </sheetPr>
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16966,8 +16966,8 @@
   </sheetPr>
   <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
paso archivos para linux
</commit_message>
<xml_diff>
--- a/compWC.xlsx
+++ b/compWC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="369" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="369" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="h1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <sheet name="h8" sheetId="10" r:id="rId10"/>
     <sheet name="fluxes (2)" sheetId="11" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
   <definedNames>
     <definedName name="xdata1" localSheetId="10">ROW(OFFSET(#REF!,0,0,513,1))-19*INT((-1/2+ROW(OFFSET(#REF!,0,0,513,1)))/19)</definedName>
     <definedName name="xdata1">ROW(OFFSET(#REF!,0,0,513,1))-19*INT((-1/2+ROW(OFFSET(#REF!,0,0,513,1)))/19)</definedName>
@@ -78,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="74">
   <si>
     <t>Site</t>
   </si>
@@ -298,6 +295,9 @@
   <si>
     <t>El riesgo de rechazar la hipótesis nula H0 cuando es verdadera es de 48.83%.</t>
   </si>
+  <si>
+    <t>Sitosterol</t>
+  </si>
 </sst>
 </file>
 
@@ -308,8 +308,8 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="&quot;] &quot;0.000&quot;,&quot;;&quot;] &quot;\-0.000&quot; ,&quot;"/>
-    <numFmt numFmtId="174" formatCode="0.000&quot; [&quot;;\-0.000&quot; [&quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot;] &quot;0.000&quot;,&quot;;&quot;] &quot;\-0.000&quot; ,&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.000&quot; [&quot;;\-0.000&quot; [&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -430,10 +430,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -449,10 +449,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -558,7 +558,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:strRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -566,7 +566,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:strRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -634,7 +634,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:strRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -642,7 +642,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:strRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -657,11 +657,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="838531328"/>
-        <c:axId val="838531720"/>
+        <c:axId val="927384240"/>
+        <c:axId val="927384632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="838531328"/>
+        <c:axId val="927384240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +679,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="838531720"/>
+        <c:crossAx val="927384632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -687,7 +687,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="838531720"/>
+        <c:axId val="927384632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +715,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="838531328"/>
+        <c:crossAx val="927384240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -804,13 +804,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>9524</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
-          <xdr:colOff>3174</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
@@ -835,26 +835,15 @@
             </a:prstGeom>
             <a:noFill/>
             <a:ln w="9525">
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
             <a:extLst>
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:noFill/>
                 </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -865,43 +854,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="dw"/>
-      <sheetName val="fluxes (2)"/>
-      <sheetName val="fluxes_2"/>
-      <sheetName val="fluxes"/>
-      <sheetName val="Sediments"/>
-      <sheetName val="Ratios_HID"/>
-      <sheetName val="Ratios_HID1"/>
-      <sheetName val="%"/>
-      <sheetName val="Hoja1"/>
-      <sheetName val="Pruebas t y z (2 muestras)1"/>
-      <sheetName val="Pruebas t y z (2 muestras)"/>
-      <sheetName val="Graphs"/>
-      <sheetName val="Sheet11"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5306,8 +5258,8 @@
   <sheetPr codeName="Hoja11"/>
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
@@ -5336,7 +5288,7 @@
         <v>4.685215402989051E-6</v>
       </c>
       <c r="F1">
-        <f>E1*1000*1000</f>
+        <f t="shared" ref="F1:F25" si="0">E1*1000*1000</f>
         <v>4.6852154029890514</v>
       </c>
       <c r="I1" t="s">
@@ -5360,7 +5312,7 @@
         <v>1.3278712011056602E-6</v>
       </c>
       <c r="F2">
-        <f>E2*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>1.3278712011056601</v>
       </c>
       <c r="I2" t="s">
@@ -5384,7 +5336,7 @@
         <v>7.4326274098166173E-7</v>
       </c>
       <c r="F3">
-        <f>E3*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>0.74326274098166178</v>
       </c>
       <c r="I3" t="s">
@@ -5408,7 +5360,7 @@
         <v>1.2724470747064167E-5</v>
       </c>
       <c r="F4">
-        <f>E4*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>12.724470747064167</v>
       </c>
       <c r="I4" t="s">
@@ -5432,7 +5384,7 @@
         <v>4.7729891213659176E-5</v>
       </c>
       <c r="F5">
-        <f>E5*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>47.72989121365918</v>
       </c>
       <c r="I5" t="s">
@@ -5456,7 +5408,7 @@
         <v>2.7487738604411186E-4</v>
       </c>
       <c r="F6">
-        <f>E6*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>274.87738604411186</v>
       </c>
       <c r="I6" t="s">
@@ -5480,7 +5432,7 @@
         <v>5.7779988065022228E-4</v>
       </c>
       <c r="F7">
-        <f>E7*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>577.79988065022224</v>
       </c>
     </row>
@@ -5501,7 +5453,7 @@
         <v>9.4182516435390831E-5</v>
       </c>
       <c r="F8">
-        <f>E8*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>94.182516435390824</v>
       </c>
     </row>
@@ -5522,7 +5474,7 @@
         <v>4.3441925767516574E-5</v>
       </c>
       <c r="F9">
-        <f>E9*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>43.44192576751658</v>
       </c>
       <c r="I9" t="s">
@@ -5546,7 +5498,7 @@
         <v>1.1840313246103783E-5</v>
       </c>
       <c r="F10">
-        <f>E10*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>11.840313246103783</v>
       </c>
     </row>
@@ -5567,7 +5519,7 @@
         <v>1.0290148624724742E-5</v>
       </c>
       <c r="F11">
-        <f>E11*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>10.290148624724742</v>
       </c>
       <c r="I11" t="s">
@@ -5591,7 +5543,7 @@
         <v>4.4908264172375392E-6</v>
       </c>
       <c r="F12">
-        <f>E12*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>4.4908264172375398</v>
       </c>
       <c r="I12" s="15">
@@ -5618,7 +5570,7 @@
         <v>5.2180898622838242E-5</v>
       </c>
       <c r="F13">
-        <f>E13*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>52.180898622838242</v>
       </c>
     </row>
@@ -5639,7 +5591,7 @@
         <v>8.596779272686035E-5</v>
       </c>
       <c r="F14">
-        <f>E14*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>85.967792726860353</v>
       </c>
       <c r="G14" s="9">
@@ -5670,7 +5622,7 @@
         <v>3.8707544530847924E-6</v>
       </c>
       <c r="F15">
-        <f>E15*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>3.8707544530847926</v>
       </c>
       <c r="G15" s="9">
@@ -5701,7 +5653,7 @@
         <v>2.0280606643491885E-4</v>
       </c>
       <c r="F16">
-        <f>E16*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>202.80606643491885</v>
       </c>
       <c r="G16" s="9"/>
@@ -5729,7 +5681,7 @@
         <v>1.3666216570398608E-4</v>
       </c>
       <c r="F17">
-        <f>E17*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>136.66216570398609</v>
       </c>
       <c r="G17" s="9"/>
@@ -5757,7 +5709,7 @@
         <v>8.6634429740125092E-6</v>
       </c>
       <c r="F18">
-        <f>E18*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>8.6634429740125096</v>
       </c>
       <c r="G18" s="9"/>
@@ -5785,7 +5737,7 @@
         <v>1.6055153950251774E-6</v>
       </c>
       <c r="F19">
-        <f>E19*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>1.6055153950251773</v>
       </c>
       <c r="G19" s="9"/>
@@ -5807,7 +5759,7 @@
         <v>5.673012500191902E-5</v>
       </c>
       <c r="F20">
-        <f>E20*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>56.730125001919021</v>
       </c>
       <c r="G20" s="9"/>
@@ -5832,7 +5784,7 @@
         <v>5.2098667271396877E-5</v>
       </c>
       <c r="F21">
-        <f>E21*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>52.098667271396877</v>
       </c>
       <c r="G21" s="9"/>
@@ -5857,7 +5809,7 @@
         <v>2.4313631189024146E-5</v>
       </c>
       <c r="F22">
-        <f>E22*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>24.313631189024147</v>
       </c>
       <c r="G22" s="9"/>
@@ -5882,7 +5834,7 @@
         <v>4.3009951419956771E-6</v>
       </c>
       <c r="F23">
-        <f>E23*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>4.3009951419956778</v>
       </c>
       <c r="G23" s="9"/>
@@ -5907,7 +5859,7 @@
         <v>8.1733805093150199E-6</v>
       </c>
       <c r="F24">
-        <f>E24*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>8.1733805093150202</v>
       </c>
       <c r="G24" s="9"/>
@@ -5932,7 +5884,7 @@
         <v>3.4913174280469657E-5</v>
       </c>
       <c r="F25">
-        <f>E25*1000*1000</f>
+        <f t="shared" si="0"/>
         <v>34.913174280469661</v>
       </c>
       <c r="G25" s="9"/>
@@ -8108,10 +8060,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:AKG43"/>
+  <dimension ref="A1:AKF43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8127,8 +8079,8 @@
     <col min="12" max="15" width="8.85546875" style="1"/>
     <col min="16" max="16" width="9.42578125" style="1"/>
     <col min="17" max="17" width="12.140625" style="2"/>
-    <col min="18" max="969" width="7" style="1"/>
-    <col min="970" max="1025" width="8.5703125"/>
+    <col min="18" max="968" width="7" style="1"/>
+    <col min="969" max="1024" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -8148,7 +8100,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -8418,7 +8370,7 @@
         <v>26259.724896443298</v>
       </c>
       <c r="F6" s="1">
-        <v>600.36497499999996</v>
+        <v>688.4079999999999</v>
       </c>
       <c r="G6" s="1">
         <v>3724.7342229999999</v>
@@ -8472,7 +8424,7 @@
         <v>12691.585503083001</v>
       </c>
       <c r="F7" s="1">
-        <v>247.12909999999999</v>
+        <v>828.46690000000001</v>
       </c>
       <c r="G7" s="1">
         <v>1255.9416719999999</v>
@@ -8526,7 +8478,7 @@
         <v>3814.3829999999998</v>
       </c>
       <c r="F8" s="1">
-        <v>201.61</v>
+        <v>212.81</v>
       </c>
       <c r="G8" s="1">
         <v>522.17169999999999</v>
@@ -8688,7 +8640,7 @@
         <v>24218.127503994001</v>
       </c>
       <c r="F11" s="1">
-        <v>453.97522099999998</v>
+        <v>509.953329</v>
       </c>
       <c r="G11" s="1">
         <v>2688.9137660000001</v>
@@ -8796,7 +8748,7 @@
         <v>13343.2080594608</v>
       </c>
       <c r="F13" s="1">
-        <v>263.32073250000002</v>
+        <v>285.98795749999999</v>
       </c>
       <c r="G13" s="1">
         <v>1362.692777</v>
@@ -9390,7 +9342,7 @@
         <v>31.735401800000002</v>
       </c>
       <c r="F24" s="1">
-        <v>8.2639999999999993</v>
+        <v>9.2134</v>
       </c>
       <c r="G24" s="1">
         <v>7.2359999999999998</v>
@@ -9444,7 +9396,7 @@
         <v>89.350499999999997</v>
       </c>
       <c r="F25" s="1">
-        <v>26.3</v>
+        <v>28.344999999999999</v>
       </c>
       <c r="G25" s="1">
         <v>25.45</v>
@@ -9498,7 +9450,7 @@
         <v>74.158659999999998</v>
       </c>
       <c r="F26" s="1">
-        <v>19.521000000000001</v>
+        <v>20.4755</v>
       </c>
       <c r="G26" s="1">
         <v>31.215</v>
@@ -9606,7 +9558,7 @@
         <v>17.767846191740102</v>
       </c>
       <c r="F28" s="1">
-        <v>2.04365164584065</v>
+        <v>3.3542834753235198</v>
       </c>
       <c r="G28" s="1">
         <v>3.9194273204057501</v>
@@ -9822,7 +9774,7 @@
         <v>28.476289767863001</v>
       </c>
       <c r="F32" s="1">
-        <v>6.7912604514958899</v>
+        <v>8.4649223555358191</v>
       </c>
       <c r="G32" s="1">
         <v>6.7424888010969601</v>
@@ -10416,7 +10368,7 @@
         <v>31.015589380579598</v>
       </c>
       <c r="F43" s="1">
-        <v>6.5336873467280396</v>
+        <v>6.5527243041727274</v>
       </c>
       <c r="G43" s="1">
         <v>3.61793576248273</v>
@@ -10464,8 +10416,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10737,7 +10689,7 @@
         <v>26259.724896443298</v>
       </c>
       <c r="E6" s="1">
-        <v>600.36497499999996</v>
+        <v>688.4079999999999</v>
       </c>
       <c r="F6" s="1">
         <v>3724.7342229999999</v>
@@ -10787,7 +10739,7 @@
         <v>12691.585503083001</v>
       </c>
       <c r="E7" s="1">
-        <v>247.12909999999999</v>
+        <v>828.46690000000001</v>
       </c>
       <c r="F7" s="1">
         <v>1255.9416719999999</v>
@@ -10837,7 +10789,7 @@
         <v>3814.3829999999998</v>
       </c>
       <c r="E8" s="1">
-        <v>201.61</v>
+        <v>212.81</v>
       </c>
       <c r="F8" s="1">
         <v>522.17169999999999</v>
@@ -10987,7 +10939,7 @@
         <v>24218.127503994001</v>
       </c>
       <c r="E11" s="1">
-        <v>453.97522099999998</v>
+        <v>509.953329</v>
       </c>
       <c r="F11" s="1">
         <v>2688.9137660000001</v>
@@ -11087,7 +11039,7 @@
         <v>13343.2080594608</v>
       </c>
       <c r="E13" s="1">
-        <v>263.32073250000002</v>
+        <v>285.98795749999999</v>
       </c>
       <c r="F13" s="1">
         <v>1362.692777</v>
@@ -11637,7 +11589,7 @@
         <v>31.735401800000002</v>
       </c>
       <c r="E24" s="1">
-        <v>8.2639999999999993</v>
+        <v>9.2134</v>
       </c>
       <c r="F24" s="1">
         <v>7.2359999999999998</v>
@@ -11687,7 +11639,7 @@
         <v>89.350499999999997</v>
       </c>
       <c r="E25" s="1">
-        <v>26.3</v>
+        <v>28.344999999999999</v>
       </c>
       <c r="F25" s="1">
         <v>25.45</v>
@@ -11737,7 +11689,7 @@
         <v>74.158659999999998</v>
       </c>
       <c r="E26" s="1">
-        <v>19.521000000000001</v>
+        <v>20.4755</v>
       </c>
       <c r="F26" s="1">
         <v>31.215</v>
@@ -11837,7 +11789,7 @@
         <v>17.767846191740102</v>
       </c>
       <c r="E28" s="1">
-        <v>2.04365164584065</v>
+        <v>3.3542834753235198</v>
       </c>
       <c r="F28" s="1">
         <v>3.9194273204057501</v>
@@ -12037,7 +11989,7 @@
         <v>28.476289767863001</v>
       </c>
       <c r="E32" s="1">
-        <v>6.7912604514958899</v>
+        <v>8.4649223555358191</v>
       </c>
       <c r="F32" s="1">
         <v>6.7424888010969601</v>
@@ -12587,7 +12539,7 @@
         <v>31.015589380579598</v>
       </c>
       <c r="E43" s="1">
-        <v>6.5336873467280396</v>
+        <v>6.5527243041727274</v>
       </c>
       <c r="F43" s="1">
         <v>3.61793576248273</v>
@@ -17069,7 +17021,7 @@
         <v>22.306671918433999</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F65" si="1">G34-E34-D34-C34</f>
+        <f t="shared" ref="F34:F58" si="1">G34-E34-D34-C34</f>
         <v>1.3585407278612038</v>
       </c>
       <c r="G34">

</xml_diff>